<commit_message>
Pt DVM corrections, etc
Added Pt resistance corrections (for each corrected raw reading). Each
reading is converted to a temperature (plus a temperature definition)
and then the average of the resulting temperatures is used to correct
the value of Rs.
Reduced delay at end of each cycle from 5s to 0.5 s.
Tidied-up Uncertainize() fn.
Fixed bug in gain_err() fn where default nomV and nomRange ('01')
assigned wrongly.

Also ensure analysis results widgets are blank before analyzing.
</commit_message>
<xml_diff>
--- a/IVY_template.xlsx
+++ b/IVY_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27585" windowHeight="12150" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27585" windowHeight="12150" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Comments" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="448">
   <si>
     <t>WARNING: DO NOT INSERT ANY COMMENTS IN THIS WORKBOOK!</t>
   </si>
@@ -1438,13 +1438,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF5B9BD5"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF5B9BD5"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1854,11 +1854,11 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2539,12 +2539,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T72"/>
+  <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="570"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="570" topLeftCell="A2"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="S28" sqref="S28"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2588,132 +2588,78 @@
         <v>41</v>
       </c>
       <c r="B1" s="41">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B4" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C4" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D4" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E4" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F4" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G4" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H4" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I4" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J4" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="K4" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="L3" s="42" t="s">
+      <c r="L4" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="42" t="s">
+      <c r="M4" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="N4" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="O4" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="42" t="s">
+      <c r="P4" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="42" t="s">
+      <c r="Q4" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="R3" s="42" t="s">
+      <c r="R4" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="S3" s="42" t="s">
+      <c r="S4" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="T3" s="42" t="s">
+      <c r="T4" s="42" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="43">
-        <v>100000</v>
-      </c>
-      <c r="C4" s="43">
-        <v>1000000</v>
-      </c>
-      <c r="D4" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="43">
-        <v>20</v>
-      </c>
-      <c r="G4" s="43">
-        <v>0</v>
-      </c>
-      <c r="H4" s="43">
-        <v>1.6535424532024291E-7</v>
-      </c>
-      <c r="I4" s="43">
-        <v>9.7688432724200655E-7</v>
-      </c>
-      <c r="J4" s="43">
-        <v>5.8994792309264883E-7</v>
-      </c>
-      <c r="K4" s="43">
-        <v>8.7929679961471322E-7</v>
-      </c>
-      <c r="L4" s="43">
-        <v>20.692485416301182</v>
-      </c>
-      <c r="M4" s="43">
-        <v>108.0185169071211</v>
-      </c>
-      <c r="N4" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="O4" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="P4" s="43">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="43">
-        <v>0</v>
-      </c>
-      <c r="R4" s="43">
-        <v>0</v>
-      </c>
-      <c r="S4" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="T4" s="45" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -2730,31 +2676,31 @@
         <v>62</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F5" s="43">
         <v>20</v>
       </c>
       <c r="G5" s="43">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="43">
-        <v>-9.9999439991386441E-2</v>
+        <v>1.6535424532024291E-7</v>
       </c>
       <c r="I5" s="43">
-        <v>1.300200516809876E-6</v>
+        <v>9.7688432724200655E-7</v>
       </c>
       <c r="J5" s="43">
-        <v>0.99999809712941945</v>
+        <v>5.8994792309264883E-7</v>
       </c>
       <c r="K5" s="43">
-        <v>8.7407328542997039E-6</v>
+        <v>8.7929679961471322E-7</v>
       </c>
       <c r="L5" s="43">
-        <v>20.924065264809141</v>
+        <v>20.692485416301182</v>
       </c>
       <c r="M5" s="43">
-        <v>108.00441117682421</v>
+        <v>108.0185169071211</v>
       </c>
       <c r="N5" s="43" t="s">
         <v>64</v>
@@ -2771,11 +2717,11 @@
       <c r="R5" s="43">
         <v>0</v>
       </c>
-      <c r="S5" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="T5" s="47" t="s">
-        <v>70</v>
+      <c r="S5" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="T5" s="45" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -2792,31 +2738,31 @@
         <v>62</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F6" s="43">
         <v>20</v>
       </c>
       <c r="G6" s="43">
-        <v>0.1</v>
+        <v>-0.1</v>
       </c>
       <c r="H6" s="43">
-        <v>0.1000001989083857</v>
+        <v>-9.9999439991386441E-2</v>
       </c>
       <c r="I6" s="43">
-        <v>1.9723465020487489E-6</v>
+        <v>1.300200516809876E-6</v>
       </c>
       <c r="J6" s="43">
-        <v>-1.0000060211258319</v>
+        <v>0.99999809712941945</v>
       </c>
       <c r="K6" s="43">
-        <v>1.163884870630302E-5</v>
+        <v>8.7407328542997039E-6</v>
       </c>
       <c r="L6" s="43">
-        <v>20.168912867133681</v>
+        <v>20.924065264809141</v>
       </c>
       <c r="M6" s="43">
-        <v>108.00647674160309</v>
+        <v>108.00441117682421</v>
       </c>
       <c r="N6" s="43" t="s">
         <v>64</v>
@@ -2834,10 +2780,10 @@
         <v>0</v>
       </c>
       <c r="S6" s="46" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="T6" s="47" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -2854,31 +2800,31 @@
         <v>62</v>
       </c>
       <c r="E7" s="43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F7" s="43">
         <v>20</v>
       </c>
       <c r="G7" s="43">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="43">
-        <v>1.177279267328127E-7</v>
+        <v>0.1000001989083857</v>
       </c>
       <c r="I7" s="43">
-        <v>1.166557267799614E-6</v>
+        <v>1.9723465020487489E-6</v>
       </c>
       <c r="J7" s="43">
-        <v>2.3918806027091302E-7</v>
+        <v>-1.0000060211258319</v>
       </c>
       <c r="K7" s="43">
-        <v>9.1108753075651978E-7</v>
+        <v>1.163884870630302E-5</v>
       </c>
       <c r="L7" s="43">
-        <v>20.435032394119691</v>
+        <v>20.168912867133681</v>
       </c>
       <c r="M7" s="43">
-        <v>107.98807285909569</v>
+        <v>108.00647674160309</v>
       </c>
       <c r="N7" s="43" t="s">
         <v>64</v>
@@ -2896,10 +2842,10 @@
         <v>0</v>
       </c>
       <c r="S7" s="46" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="T7" s="47" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -2913,10 +2859,10 @@
         <v>1000000</v>
       </c>
       <c r="D8" s="43" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F8" s="43">
         <v>20</v>
@@ -2924,23 +2870,23 @@
       <c r="G8" s="43">
         <v>0</v>
       </c>
-      <c r="H8" s="48">
-        <v>2.2082467508196881E-8</v>
-      </c>
-      <c r="I8" s="48">
-        <v>1.0098484535640989E-6</v>
+      <c r="H8" s="43">
+        <v>1.177279267328127E-7</v>
+      </c>
+      <c r="I8" s="43">
+        <v>1.166557267799614E-6</v>
       </c>
       <c r="J8" s="43">
-        <v>9.4775663456321606E-8</v>
+        <v>2.3918806027091302E-7</v>
       </c>
       <c r="K8" s="43">
-        <v>8.3457170550847248E-7</v>
+        <v>9.1108753075651978E-7</v>
       </c>
       <c r="L8" s="43">
-        <v>20.433720709072318</v>
+        <v>20.435032394119691</v>
       </c>
       <c r="M8" s="43">
-        <v>107.9890847207639</v>
+        <v>107.98807285909569</v>
       </c>
       <c r="N8" s="43" t="s">
         <v>64</v>
@@ -2958,10 +2904,10 @@
         <v>0</v>
       </c>
       <c r="S8" s="46" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="T8" s="47" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -2978,31 +2924,31 @@
         <v>77</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F9" s="43">
         <v>20</v>
       </c>
       <c r="G9" s="43">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="48">
-        <v>-0.1000001769921381</v>
+        <v>2.2082467508196881E-8</v>
       </c>
       <c r="I9" s="48">
-        <v>1.6866651411321669E-6</v>
+        <v>1.0098484535640989E-6</v>
       </c>
       <c r="J9" s="43">
-        <v>4.6912897761383359E-8</v>
+        <v>9.4775663456321606E-8</v>
       </c>
       <c r="K9" s="43">
-        <v>1.1027399294090279E-5</v>
+        <v>8.3457170550847248E-7</v>
       </c>
       <c r="L9" s="43">
-        <v>20.829860612736411</v>
+        <v>20.433720709072318</v>
       </c>
       <c r="M9" s="43">
-        <v>108.0117667347447</v>
+        <v>107.9890847207639</v>
       </c>
       <c r="N9" s="43" t="s">
         <v>64</v>
@@ -3020,10 +2966,10 @@
         <v>0</v>
       </c>
       <c r="S9" s="46" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T9" s="47" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -3040,31 +2986,31 @@
         <v>77</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F10" s="43">
         <v>20</v>
       </c>
       <c r="G10" s="43">
-        <v>0.1</v>
+        <v>-0.1</v>
       </c>
       <c r="H10" s="48">
-        <v>0.1000002120763536</v>
+        <v>-0.1000001769921381</v>
       </c>
       <c r="I10" s="48">
-        <v>1.7232909951508961E-6</v>
+        <v>1.6866651411321669E-6</v>
       </c>
       <c r="J10" s="43">
-        <v>2.2379161260586329E-6</v>
+        <v>4.6912897761383359E-8</v>
       </c>
       <c r="K10" s="43">
-        <v>1.132879999918373E-5</v>
+        <v>1.1027399294090279E-5</v>
       </c>
       <c r="L10" s="43">
-        <v>20.60359925673907</v>
+        <v>20.829860612736411</v>
       </c>
       <c r="M10" s="43">
-        <v>107.9977602478789</v>
+        <v>108.0117667347447</v>
       </c>
       <c r="N10" s="43" t="s">
         <v>64</v>
@@ -3081,11 +3027,11 @@
       <c r="R10" s="43">
         <v>0</v>
       </c>
-      <c r="S10" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="T10" s="50" t="s">
-        <v>86</v>
+      <c r="S10" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="T10" s="47" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -3102,31 +3048,31 @@
         <v>77</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F11" s="43">
         <v>20</v>
       </c>
       <c r="G11" s="43">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H11" s="48">
-        <v>-3.2849313129488311E-8</v>
+        <v>0.1000002120763536</v>
       </c>
       <c r="I11" s="48">
-        <v>8.4055265051731195E-7</v>
+        <v>1.7232909951508961E-6</v>
       </c>
       <c r="J11" s="43">
-        <v>4.9081735525558836E-7</v>
+        <v>2.2379161260586329E-6</v>
       </c>
       <c r="K11" s="43">
-        <v>9.4880851890355726E-7</v>
+        <v>1.132879999918373E-5</v>
       </c>
       <c r="L11" s="43">
-        <v>20.82978297651357</v>
+        <v>20.60359925673907</v>
       </c>
       <c r="M11" s="43">
-        <v>107.9989811575978</v>
+        <v>107.9977602478789</v>
       </c>
       <c r="N11" s="43" t="s">
         <v>64</v>
@@ -3143,60 +3089,66 @@
       <c r="R11" s="43">
         <v>0</v>
       </c>
+      <c r="S11" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="T11" s="50" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="51">
+      <c r="B12" s="43">
         <v>100000</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12" s="43">
         <v>1000000</v>
       </c>
-      <c r="D12" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="51">
+      <c r="D12" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="43">
         <v>20</v>
       </c>
-      <c r="G12" s="51">
-        <v>0</v>
-      </c>
-      <c r="H12" s="51">
-        <v>1.043230180901704E-7</v>
-      </c>
-      <c r="I12" s="51">
-        <v>1.0608040662726161E-6</v>
-      </c>
-      <c r="J12" s="51">
-        <v>5.1191618520369837E-7</v>
-      </c>
-      <c r="K12" s="51">
-        <v>1.14982568578084E-6</v>
-      </c>
-      <c r="L12" s="51">
-        <v>20.60520775345918</v>
-      </c>
-      <c r="M12" s="51">
-        <v>107.9903585779613</v>
-      </c>
-      <c r="N12" s="51" t="s">
+      <c r="G12" s="43">
+        <v>0</v>
+      </c>
+      <c r="H12" s="48">
+        <v>-3.2849313129488311E-8</v>
+      </c>
+      <c r="I12" s="48">
+        <v>8.4055265051731195E-7</v>
+      </c>
+      <c r="J12" s="43">
+        <v>4.9081735525558836E-7</v>
+      </c>
+      <c r="K12" s="43">
+        <v>9.4880851890355726E-7</v>
+      </c>
+      <c r="L12" s="43">
+        <v>20.82978297651357</v>
+      </c>
+      <c r="M12" s="43">
+        <v>107.9989811575978</v>
+      </c>
+      <c r="N12" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="O12" s="51" t="s">
+      <c r="O12" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="P12" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="51">
-        <v>0</v>
-      </c>
-      <c r="R12" s="51">
+      <c r="P12" s="43">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="43">
+        <v>0</v>
+      </c>
+      <c r="R12" s="43">
         <v>0</v>
       </c>
     </row>
@@ -3214,31 +3166,31 @@
         <v>62</v>
       </c>
       <c r="E13" s="51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="51">
         <v>20</v>
       </c>
       <c r="G13" s="51">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="51">
-        <v>-0.99999843680342448</v>
+        <v>1.043230180901704E-7</v>
       </c>
       <c r="I13" s="51">
-        <v>8.8403107877673053E-6</v>
+        <v>1.0608040662726161E-6</v>
       </c>
       <c r="J13" s="51">
-        <v>9.9999844063238861</v>
+        <v>5.1191618520369837E-7</v>
       </c>
       <c r="K13" s="51">
-        <v>9.71969135228006E-5</v>
+        <v>1.14982568578084E-6</v>
       </c>
       <c r="L13" s="51">
-        <v>20.540717916196211</v>
+        <v>20.60520775345918</v>
       </c>
       <c r="M13" s="51">
-        <v>108.0035156101641</v>
+        <v>107.9903585779613</v>
       </c>
       <c r="N13" s="51" t="s">
         <v>64</v>
@@ -3270,31 +3222,31 @@
         <v>62</v>
       </c>
       <c r="E14" s="51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F14" s="51">
         <v>20</v>
       </c>
       <c r="G14" s="51">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H14" s="51">
-        <v>0.99999928537714777</v>
+        <v>-0.99999843680342448</v>
       </c>
       <c r="I14" s="51">
-        <v>1.0604426471689379E-5</v>
+        <v>8.8403107877673053E-6</v>
       </c>
       <c r="J14" s="51">
-        <v>-10.00002626818541</v>
+        <v>9.9999844063238861</v>
       </c>
       <c r="K14" s="51">
-        <v>1.042166915049861E-4</v>
+        <v>9.71969135228006E-5</v>
       </c>
       <c r="L14" s="51">
-        <v>20.4940823493096</v>
+        <v>20.540717916196211</v>
       </c>
       <c r="M14" s="51">
-        <v>108.0103013646265</v>
+        <v>108.0035156101641</v>
       </c>
       <c r="N14" s="51" t="s">
         <v>64</v>
@@ -3326,31 +3278,31 @@
         <v>62</v>
       </c>
       <c r="E15" s="51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F15" s="51">
         <v>20</v>
       </c>
       <c r="G15" s="51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="51">
-        <v>1.7908888342222789E-7</v>
+        <v>0.99999928537714777</v>
       </c>
       <c r="I15" s="51">
-        <v>8.1449345389520547E-7</v>
+        <v>1.0604426471689379E-5</v>
       </c>
       <c r="J15" s="51">
-        <v>3.3608501923704182E-7</v>
+        <v>-10.00002626818541</v>
       </c>
       <c r="K15" s="51">
-        <v>8.0930156436342921E-7</v>
+        <v>1.042166915049861E-4</v>
       </c>
       <c r="L15" s="51">
-        <v>20.63703553166863</v>
+        <v>20.4940823493096</v>
       </c>
       <c r="M15" s="51">
-        <v>107.9903939140209</v>
+        <v>108.0103013646265</v>
       </c>
       <c r="N15" s="51" t="s">
         <v>64</v>
@@ -3379,10 +3331,10 @@
         <v>1000000</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E16" s="51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F16" s="51">
         <v>20</v>
@@ -3390,23 +3342,23 @@
       <c r="G16" s="51">
         <v>0</v>
       </c>
-      <c r="H16" s="52">
-        <v>2.9577520849956949E-8</v>
-      </c>
-      <c r="I16" s="52">
-        <v>8.5164956906876791E-7</v>
+      <c r="H16" s="51">
+        <v>1.7908888342222789E-7</v>
+      </c>
+      <c r="I16" s="51">
+        <v>8.1449345389520547E-7</v>
       </c>
       <c r="J16" s="51">
-        <v>-2.7182644622249209E-7</v>
+        <v>3.3608501923704182E-7</v>
       </c>
       <c r="K16" s="51">
-        <v>9.2078119864429172E-7</v>
+        <v>8.0930156436342921E-7</v>
       </c>
       <c r="L16" s="51">
-        <v>20.58404391553659</v>
+        <v>20.63703553166863</v>
       </c>
       <c r="M16" s="51">
-        <v>108.0192472233577</v>
+        <v>107.9903939140209</v>
       </c>
       <c r="N16" s="51" t="s">
         <v>64</v>
@@ -3438,31 +3390,31 @@
         <v>77</v>
       </c>
       <c r="E17" s="51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F17" s="51">
         <v>20</v>
       </c>
       <c r="G17" s="51">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="52">
-        <v>-0.99999902245261585</v>
+        <v>2.9577520849956949E-8</v>
       </c>
       <c r="I17" s="52">
-        <v>9.6011699550175887E-6</v>
+        <v>8.5164956906876791E-7</v>
       </c>
       <c r="J17" s="51">
-        <v>1.488685015948713E-5</v>
+        <v>-2.7182644622249209E-7</v>
       </c>
       <c r="K17" s="51">
-        <v>1.005786994378101E-4</v>
+        <v>9.2078119864429172E-7</v>
       </c>
       <c r="L17" s="51">
-        <v>20.607029971716461</v>
+        <v>20.58404391553659</v>
       </c>
       <c r="M17" s="51">
-        <v>108.0205022301015</v>
+        <v>108.0192472233577</v>
       </c>
       <c r="N17" s="51" t="s">
         <v>64</v>
@@ -3494,31 +3446,31 @@
         <v>77</v>
       </c>
       <c r="E18" s="51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F18" s="51">
         <v>20</v>
       </c>
       <c r="G18" s="51">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H18" s="52">
-        <v>1.0000033399565471</v>
+        <v>-0.99999902245261585</v>
       </c>
       <c r="I18" s="52">
-        <v>9.8845436395903917E-6</v>
+        <v>9.6011699550175887E-6</v>
       </c>
       <c r="J18" s="51">
-        <v>1.0788730309276109E-6</v>
+        <v>1.488685015948713E-5</v>
       </c>
       <c r="K18" s="51">
-        <v>1.182261489900015E-4</v>
+        <v>1.005786994378101E-4</v>
       </c>
       <c r="L18" s="51">
-        <v>20.542748618959781</v>
+        <v>20.607029971716461</v>
       </c>
       <c r="M18" s="51">
-        <v>107.98501545838811</v>
+        <v>108.0205022301015</v>
       </c>
       <c r="N18" s="51" t="s">
         <v>64</v>
@@ -3550,31 +3502,31 @@
         <v>77</v>
       </c>
       <c r="E19" s="51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F19" s="51">
         <v>20</v>
       </c>
       <c r="G19" s="51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="52">
-        <v>3.1739890739093477E-8</v>
+        <v>1.0000033399565471</v>
       </c>
       <c r="I19" s="52">
-        <v>1.236115749832685E-6</v>
+        <v>9.8845436395903917E-6</v>
       </c>
       <c r="J19" s="51">
-        <v>-9.5668684700356169E-8</v>
+        <v>1.0788730309276109E-6</v>
       </c>
       <c r="K19" s="51">
-        <v>1.024369905438836E-6</v>
+        <v>1.182261489900015E-4</v>
       </c>
       <c r="L19" s="51">
-        <v>20.202994679432251</v>
+        <v>20.542748618959781</v>
       </c>
       <c r="M19" s="51">
-        <v>108.0110584172352</v>
+        <v>107.98501545838811</v>
       </c>
       <c r="N19" s="51" t="s">
         <v>64</v>
@@ -3593,197 +3545,129 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="51">
+        <v>100000</v>
+      </c>
+      <c r="C20" s="51">
+        <v>1000000</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="51">
+        <v>20</v>
+      </c>
+      <c r="G20" s="51">
+        <v>0</v>
+      </c>
+      <c r="H20" s="52">
+        <v>3.1739890739093477E-8</v>
+      </c>
+      <c r="I20" s="52">
+        <v>1.236115749832685E-6</v>
+      </c>
+      <c r="J20" s="51">
+        <v>-9.5668684700356169E-8</v>
+      </c>
+      <c r="K20" s="51">
+        <v>1.024369905438836E-6</v>
+      </c>
+      <c r="L20" s="51">
+        <v>20.202994679432251</v>
+      </c>
+      <c r="M20" s="51">
+        <v>108.0110584172352</v>
+      </c>
+      <c r="N20" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="O20" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="P20" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="51">
+        <v>0</v>
+      </c>
+      <c r="R20" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B22" s="10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B23" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C23" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D23" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E23" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="F23" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="G21" s="42" t="s">
+      <c r="G23" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="H21" s="42" t="s">
+      <c r="H23" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="I21" s="42" t="s">
+      <c r="I23" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="J21" s="42" t="s">
+      <c r="J23" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="42" t="s">
+      <c r="K23" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="L21" s="42" t="s">
+      <c r="L23" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="M21" s="42" t="s">
+      <c r="M23" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="N21" s="42" t="s">
+      <c r="N23" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="O21" s="42" t="s">
+      <c r="O23" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="P21" s="42" t="s">
+      <c r="P23" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="Q21" s="42" t="s">
+      <c r="Q23" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="R21" s="42" t="s">
+      <c r="R23" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="S21" s="42" t="s">
+      <c r="S23" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="T21" s="42" t="s">
+      <c r="T23" s="42" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="43">
-        <v>1000000</v>
-      </c>
-      <c r="C22" s="43">
-        <v>1000000</v>
-      </c>
-      <c r="D22" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="F22" s="43">
-        <v>20</v>
-      </c>
-      <c r="G22" s="43">
-        <v>0</v>
-      </c>
-      <c r="H22" s="43">
-        <v>-7.0862656918973481E-8</v>
-      </c>
-      <c r="I22" s="43">
-        <v>8.2492141911443321E-7</v>
-      </c>
-      <c r="J22" s="43">
-        <v>-1.157637159856024E-7</v>
-      </c>
-      <c r="K22" s="43">
-        <v>8.3532706611426517E-7</v>
-      </c>
-      <c r="L22" s="43">
-        <v>20.616075090724991</v>
-      </c>
-      <c r="M22" s="43">
-        <v>107.9997017067486</v>
-      </c>
-      <c r="N22" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="O22" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="P22" s="43">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="43">
-        <v>0</v>
-      </c>
-      <c r="R22" s="43">
-        <v>0</v>
-      </c>
-      <c r="S22" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="T22" s="54" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" s="43">
-        <v>1000000</v>
-      </c>
-      <c r="C23" s="43">
-        <v>1000000</v>
-      </c>
-      <c r="D23" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="43">
-        <v>20</v>
-      </c>
-      <c r="G23" s="43">
-        <v>-0.1</v>
-      </c>
-      <c r="H23" s="43">
-        <v>-9.9999954294226007E-2</v>
-      </c>
-      <c r="I23" s="43">
-        <v>2.2609456749623549E-6</v>
-      </c>
-      <c r="J23" s="43">
-        <v>9.9999358003854816E-2</v>
-      </c>
-      <c r="K23" s="43">
-        <v>1.9142600856871258E-6</v>
-      </c>
-      <c r="L23" s="43">
-        <v>20.408543991795661</v>
-      </c>
-      <c r="M23" s="43">
-        <v>108.0044527985402</v>
-      </c>
-      <c r="N23" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="O23" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="P23" s="43">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="43">
-        <v>0</v>
-      </c>
-      <c r="R23" s="43">
-        <v>0</v>
-      </c>
-      <c r="S23" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="T23" s="56" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -3800,31 +3684,31 @@
         <v>62</v>
       </c>
       <c r="E24" s="43" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F24" s="43">
         <v>20</v>
       </c>
       <c r="G24" s="43">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="43">
-        <v>9.9999810128103883E-2</v>
+        <v>-7.0862656918973481E-8</v>
       </c>
       <c r="I24" s="43">
-        <v>1.9844997561831732E-6</v>
+        <v>8.2492141911443321E-7</v>
       </c>
       <c r="J24" s="43">
-        <v>-0.1000001362415924</v>
+        <v>-1.157637159856024E-7</v>
       </c>
       <c r="K24" s="43">
-        <v>2.3091683416907639E-6</v>
+        <v>8.3532706611426517E-7</v>
       </c>
       <c r="L24" s="43">
-        <v>21.186343527593291</v>
+        <v>20.616075090724991</v>
       </c>
       <c r="M24" s="43">
-        <v>107.99444747209419</v>
+        <v>107.9997017067486</v>
       </c>
       <c r="N24" s="43" t="s">
         <v>64</v>
@@ -3841,11 +3725,11 @@
       <c r="R24" s="43">
         <v>0</v>
       </c>
-      <c r="S24" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="T24" s="56" t="s">
-        <v>73</v>
+      <c r="S24" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="T24" s="54" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -3862,31 +3746,31 @@
         <v>62</v>
       </c>
       <c r="E25" s="43" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F25" s="43">
         <v>20</v>
       </c>
       <c r="G25" s="43">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="H25" s="43">
-        <v>-2.9546741621585182E-7</v>
+        <v>-9.9999954294226007E-2</v>
       </c>
       <c r="I25" s="43">
-        <v>9.312016313094661E-7</v>
+        <v>2.2609456749623549E-6</v>
       </c>
       <c r="J25" s="43">
-        <v>-1.9410849686831329E-8</v>
+        <v>9.9999358003854816E-2</v>
       </c>
       <c r="K25" s="43">
-        <v>7.5705403987838191E-7</v>
+        <v>1.9142600856871258E-6</v>
       </c>
       <c r="L25" s="43">
-        <v>20.64232356446734</v>
+        <v>20.408543991795661</v>
       </c>
       <c r="M25" s="43">
-        <v>107.9988862169257</v>
+        <v>108.0044527985402</v>
       </c>
       <c r="N25" s="43" t="s">
         <v>64</v>
@@ -3904,10 +3788,10 @@
         <v>0</v>
       </c>
       <c r="S25" s="55" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="T25" s="56" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -3921,34 +3805,34 @@
         <v>1000000</v>
       </c>
       <c r="D26" s="43" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E26" s="43" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F26" s="43">
         <v>20</v>
       </c>
       <c r="G26" s="43">
-        <v>0</v>
-      </c>
-      <c r="H26" s="48">
-        <v>9.5344988316748626E-8</v>
-      </c>
-      <c r="I26" s="48">
-        <v>9.2998417370208525E-7</v>
+        <v>0.1</v>
+      </c>
+      <c r="H26" s="43">
+        <v>9.9999810128103883E-2</v>
+      </c>
+      <c r="I26" s="43">
+        <v>1.9844997561831732E-6</v>
       </c>
       <c r="J26" s="43">
-        <v>-2.8795600117035182E-7</v>
+        <v>-0.1000001362415924</v>
       </c>
       <c r="K26" s="43">
-        <v>1.20922822056675E-6</v>
+        <v>2.3091683416907639E-6</v>
       </c>
       <c r="L26" s="43">
-        <v>20.392837766087158</v>
+        <v>21.186343527593291</v>
       </c>
       <c r="M26" s="43">
-        <v>108.0029363279651</v>
+        <v>107.99444747209419</v>
       </c>
       <c r="N26" s="43" t="s">
         <v>64</v>
@@ -3966,10 +3850,10 @@
         <v>0</v>
       </c>
       <c r="S26" s="55" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="T26" s="56" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
@@ -3983,34 +3867,34 @@
         <v>1000000</v>
       </c>
       <c r="D27" s="43" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E27" s="43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F27" s="43">
         <v>20</v>
       </c>
       <c r="G27" s="43">
-        <v>-0.1</v>
-      </c>
-      <c r="H27" s="48">
-        <v>-9.9999961791613176E-2</v>
-      </c>
-      <c r="I27" s="48">
-        <v>2.559220592618875E-6</v>
+        <v>0</v>
+      </c>
+      <c r="H27" s="43">
+        <v>-2.9546741621585182E-7</v>
+      </c>
+      <c r="I27" s="43">
+        <v>9.312016313094661E-7</v>
       </c>
       <c r="J27" s="43">
-        <v>7.0213412539045406E-7</v>
+        <v>-1.9410849686831329E-8</v>
       </c>
       <c r="K27" s="43">
-        <v>1.6862097198378391E-6</v>
+        <v>7.5705403987838191E-7</v>
       </c>
       <c r="L27" s="43">
-        <v>20.45309345079886</v>
+        <v>20.64232356446734</v>
       </c>
       <c r="M27" s="43">
-        <v>108.0045777799895</v>
+        <v>107.9988862169257</v>
       </c>
       <c r="N27" s="43" t="s">
         <v>64</v>
@@ -4028,10 +3912,10 @@
         <v>0</v>
       </c>
       <c r="S27" s="55" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="T27" s="56" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -4048,31 +3932,31 @@
         <v>77</v>
       </c>
       <c r="E28" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F28" s="43">
         <v>20</v>
       </c>
       <c r="G28" s="43">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="48">
-        <v>0.10000017116883279</v>
+        <v>9.5344988316748626E-8</v>
       </c>
       <c r="I28" s="48">
-        <v>2.6620315140931739E-6</v>
+        <v>9.2998417370208525E-7</v>
       </c>
       <c r="J28" s="43">
-        <v>-4.6635869559315688E-7</v>
+        <v>-2.8795600117035182E-7</v>
       </c>
       <c r="K28" s="43">
-        <v>2.1306286011569889E-6</v>
+        <v>1.20922822056675E-6</v>
       </c>
       <c r="L28" s="43">
-        <v>20.382324408145699</v>
+        <v>20.392837766087158</v>
       </c>
       <c r="M28" s="43">
-        <v>107.9963009809173</v>
+        <v>108.0029363279651</v>
       </c>
       <c r="N28" s="43" t="s">
         <v>64</v>
@@ -4089,11 +3973,11 @@
       <c r="R28" s="43">
         <v>0</v>
       </c>
-      <c r="S28" s="57" t="s">
-        <v>85</v>
-      </c>
-      <c r="T28" s="58" t="s">
-        <v>86</v>
+      <c r="S28" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="T28" s="56" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -4110,31 +3994,31 @@
         <v>77</v>
       </c>
       <c r="E29" s="43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F29" s="43">
         <v>20</v>
       </c>
       <c r="G29" s="43">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="H29" s="48">
-        <v>1.872917283966511E-7</v>
+        <v>-9.9999961791613176E-2</v>
       </c>
       <c r="I29" s="48">
-        <v>8.6396092823531628E-7</v>
+        <v>2.559220592618875E-6</v>
       </c>
       <c r="J29" s="43">
-        <v>2.1772725512390919E-7</v>
+        <v>7.0213412539045406E-7</v>
       </c>
       <c r="K29" s="43">
-        <v>1.072453318140614E-6</v>
+        <v>1.6862097198378391E-6</v>
       </c>
       <c r="L29" s="43">
-        <v>20.410031726817451</v>
+        <v>20.45309345079886</v>
       </c>
       <c r="M29" s="43">
-        <v>108.0081332618611</v>
+        <v>108.0045777799895</v>
       </c>
       <c r="N29" s="43" t="s">
         <v>64</v>
@@ -4151,116 +4035,128 @@
       <c r="R29" s="43">
         <v>0</v>
       </c>
+      <c r="S29" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="T29" s="56" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="51">
+      <c r="B30" s="43">
         <v>1000000</v>
       </c>
-      <c r="C30" s="51">
+      <c r="C30" s="43">
         <v>1000000</v>
       </c>
-      <c r="D30" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" s="51">
+      <c r="D30" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="43">
         <v>20</v>
       </c>
-      <c r="G30" s="51">
-        <v>0</v>
-      </c>
-      <c r="H30" s="51">
-        <v>3.2532898363602903E-7</v>
-      </c>
-      <c r="I30" s="51">
-        <v>1.1168438182187401E-6</v>
-      </c>
-      <c r="J30" s="51">
-        <v>-1.5378274489736499E-7</v>
-      </c>
-      <c r="K30" s="51">
-        <v>1.239733242843578E-6</v>
-      </c>
-      <c r="L30" s="51">
-        <v>20.750547213812489</v>
-      </c>
-      <c r="M30" s="51">
-        <v>107.9999992080396</v>
-      </c>
-      <c r="N30" s="51" t="s">
+      <c r="G30" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="H30" s="48">
+        <v>0.10000017116883279</v>
+      </c>
+      <c r="I30" s="48">
+        <v>2.6620315140931739E-6</v>
+      </c>
+      <c r="J30" s="43">
+        <v>-4.6635869559315688E-7</v>
+      </c>
+      <c r="K30" s="43">
+        <v>2.1306286011569889E-6</v>
+      </c>
+      <c r="L30" s="43">
+        <v>20.382324408145699</v>
+      </c>
+      <c r="M30" s="43">
+        <v>107.9963009809173</v>
+      </c>
+      <c r="N30" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="O30" s="51" t="s">
+      <c r="O30" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="P30" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="51">
-        <v>0</v>
-      </c>
-      <c r="R30" s="51">
-        <v>0</v>
+      <c r="P30" s="43">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="43">
+        <v>0</v>
+      </c>
+      <c r="R30" s="43">
+        <v>0</v>
+      </c>
+      <c r="S30" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="T30" s="58" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="51">
+      <c r="B31" s="43">
         <v>1000000</v>
       </c>
-      <c r="C31" s="51">
+      <c r="C31" s="43">
         <v>1000000</v>
       </c>
-      <c r="D31" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="E31" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="F31" s="51">
+      <c r="D31" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="43">
         <v>20</v>
       </c>
-      <c r="G31" s="51">
-        <v>-1</v>
-      </c>
-      <c r="H31" s="51">
-        <v>-0.99999637364015848</v>
-      </c>
-      <c r="I31" s="51">
-        <v>1.156535093017743E-5</v>
-      </c>
-      <c r="J31" s="51">
-        <v>0.99999985476856867</v>
-      </c>
-      <c r="K31" s="51">
-        <v>9.3538267507706424E-6</v>
-      </c>
-      <c r="L31" s="51">
-        <v>20.58164174673281</v>
-      </c>
-      <c r="M31" s="51">
-        <v>107.99946468043299</v>
-      </c>
-      <c r="N31" s="51" t="s">
+      <c r="G31" s="43">
+        <v>0</v>
+      </c>
+      <c r="H31" s="48">
+        <v>1.872917283966511E-7</v>
+      </c>
+      <c r="I31" s="48">
+        <v>8.6396092823531628E-7</v>
+      </c>
+      <c r="J31" s="43">
+        <v>2.1772725512390919E-7</v>
+      </c>
+      <c r="K31" s="43">
+        <v>1.072453318140614E-6</v>
+      </c>
+      <c r="L31" s="43">
+        <v>20.410031726817451</v>
+      </c>
+      <c r="M31" s="43">
+        <v>108.0081332618611</v>
+      </c>
+      <c r="N31" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="O31" s="51" t="s">
+      <c r="O31" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="P31" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="51">
-        <v>0</v>
-      </c>
-      <c r="R31" s="51">
+      <c r="P31" s="43">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="43">
+        <v>0</v>
+      </c>
+      <c r="R31" s="43">
         <v>0</v>
       </c>
     </row>
@@ -4278,31 +4174,31 @@
         <v>62</v>
       </c>
       <c r="E32" s="51" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F32" s="51">
         <v>20</v>
       </c>
       <c r="G32" s="51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" s="51">
-        <v>1.0000009159190939</v>
+        <v>3.2532898363602903E-7</v>
       </c>
       <c r="I32" s="51">
-        <v>1.301985060063743E-5</v>
+        <v>1.1168438182187401E-6</v>
       </c>
       <c r="J32" s="51">
-        <v>-0.99999736626106461</v>
+        <v>-1.5378274489736499E-7</v>
       </c>
       <c r="K32" s="51">
-        <v>1.067330166895473E-5</v>
+        <v>1.239733242843578E-6</v>
       </c>
       <c r="L32" s="51">
-        <v>20.446838595494341</v>
+        <v>20.750547213812489</v>
       </c>
       <c r="M32" s="51">
-        <v>108.00085036857639</v>
+        <v>107.9999992080396</v>
       </c>
       <c r="N32" s="51" t="s">
         <v>64</v>
@@ -4320,7 +4216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="51" t="s">
         <v>98</v>
       </c>
@@ -4334,31 +4230,31 @@
         <v>62</v>
       </c>
       <c r="E33" s="51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F33" s="51">
         <v>20</v>
       </c>
       <c r="G33" s="51">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H33" s="51">
-        <v>2.2452433351564569E-8</v>
+        <v>-0.99999637364015848</v>
       </c>
       <c r="I33" s="51">
-        <v>1.13305898196576E-6</v>
+        <v>1.156535093017743E-5</v>
       </c>
       <c r="J33" s="51">
-        <v>1.350538800762791E-7</v>
+        <v>0.99999985476856867</v>
       </c>
       <c r="K33" s="51">
-        <v>1.1405830933669801E-6</v>
+        <v>9.3538267507706424E-6</v>
       </c>
       <c r="L33" s="51">
-        <v>20.822433065111539</v>
+        <v>20.58164174673281</v>
       </c>
       <c r="M33" s="51">
-        <v>107.99951092025481</v>
+        <v>107.99946468043299</v>
       </c>
       <c r="N33" s="51" t="s">
         <v>64</v>
@@ -4376,7 +4272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="51" t="s">
         <v>98</v>
       </c>
@@ -4387,34 +4283,34 @@
         <v>1000000</v>
       </c>
       <c r="D34" s="51" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E34" s="51" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F34" s="51">
         <v>20</v>
       </c>
       <c r="G34" s="51">
-        <v>0</v>
-      </c>
-      <c r="H34" s="52">
-        <v>-2.1262799961051439E-7</v>
-      </c>
-      <c r="I34" s="52">
-        <v>1.027654349387918E-6</v>
+        <v>1</v>
+      </c>
+      <c r="H34" s="51">
+        <v>1.0000009159190939</v>
+      </c>
+      <c r="I34" s="51">
+        <v>1.301985060063743E-5</v>
       </c>
       <c r="J34" s="51">
-        <v>1.5886936709526759E-7</v>
+        <v>-0.99999736626106461</v>
       </c>
       <c r="K34" s="51">
-        <v>1.259265733505533E-6</v>
+        <v>1.067330166895473E-5</v>
       </c>
       <c r="L34" s="51">
-        <v>20.405603240592018</v>
+        <v>20.446838595494341</v>
       </c>
       <c r="M34" s="51">
-        <v>107.99380534152</v>
+        <v>108.00085036857639</v>
       </c>
       <c r="N34" s="51" t="s">
         <v>64</v>
@@ -4432,7 +4328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="51" t="s">
         <v>98</v>
       </c>
@@ -4443,34 +4339,34 @@
         <v>1000000</v>
       </c>
       <c r="D35" s="51" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E35" s="51" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F35" s="51">
         <v>20</v>
       </c>
       <c r="G35" s="51">
-        <v>-1</v>
-      </c>
-      <c r="H35" s="52">
-        <v>-1.000000315851806</v>
-      </c>
-      <c r="I35" s="52">
-        <v>1.6701438922557101E-5</v>
+        <v>0</v>
+      </c>
+      <c r="H35" s="51">
+        <v>2.2452433351564569E-8</v>
+      </c>
+      <c r="I35" s="51">
+        <v>1.13305898196576E-6</v>
       </c>
       <c r="J35" s="51">
-        <v>1.3842157409625779E-6</v>
+        <v>1.350538800762791E-7</v>
       </c>
       <c r="K35" s="51">
-        <v>9.8166236247783203E-6</v>
+        <v>1.1405830933669801E-6</v>
       </c>
       <c r="L35" s="51">
-        <v>20.512619227195088</v>
+        <v>20.822433065111539</v>
       </c>
       <c r="M35" s="51">
-        <v>107.9963770118498</v>
+        <v>107.99951092025481</v>
       </c>
       <c r="N35" s="51" t="s">
         <v>64</v>
@@ -4488,7 +4384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="51" t="s">
         <v>98</v>
       </c>
@@ -4502,31 +4398,31 @@
         <v>77</v>
       </c>
       <c r="E36" s="51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F36" s="51">
         <v>20</v>
       </c>
       <c r="G36" s="51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" s="52">
-        <v>1.0000034004439251</v>
+        <v>-2.1262799961051439E-7</v>
       </c>
       <c r="I36" s="52">
-        <v>1.1184213772461109E-5</v>
+        <v>1.027654349387918E-6</v>
       </c>
       <c r="J36" s="51">
-        <v>-3.6803975193013112E-6</v>
+        <v>1.5886936709526759E-7</v>
       </c>
       <c r="K36" s="51">
-        <v>1.3891659195575229E-5</v>
+        <v>1.259265733505533E-6</v>
       </c>
       <c r="L36" s="51">
-        <v>20.479643918171281</v>
+        <v>20.405603240592018</v>
       </c>
       <c r="M36" s="51">
-        <v>108.00508197528789</v>
+        <v>107.99380534152</v>
       </c>
       <c r="N36" s="51" t="s">
         <v>64</v>
@@ -4544,7 +4440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="51" t="s">
         <v>98</v>
       </c>
@@ -4558,31 +4454,31 @@
         <v>77</v>
       </c>
       <c r="E37" s="51" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F37" s="51">
         <v>20</v>
       </c>
       <c r="G37" s="51">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H37" s="52">
-        <v>-9.6236139540002298E-9</v>
+        <v>-1.000000315851806</v>
       </c>
       <c r="I37" s="52">
-        <v>1.027462984734989E-6</v>
+        <v>1.6701438922557101E-5</v>
       </c>
       <c r="J37" s="51">
-        <v>-7.6384269314035401E-8</v>
+        <v>1.3842157409625779E-6</v>
       </c>
       <c r="K37" s="51">
-        <v>6.5017047333985786E-7</v>
+        <v>9.8166236247783203E-6</v>
       </c>
       <c r="L37" s="51">
-        <v>20.63494115251099</v>
+        <v>20.512619227195088</v>
       </c>
       <c r="M37" s="51">
-        <v>108.0058471423382</v>
+        <v>107.9963770118498</v>
       </c>
       <c r="N37" s="51" t="s">
         <v>64</v>
@@ -4600,119 +4496,119 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="59" t="s">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="59">
+      <c r="B38" s="51">
         <v>1000000</v>
       </c>
-      <c r="C38" s="59">
+      <c r="C38" s="51">
         <v>1000000</v>
       </c>
-      <c r="D38" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="E38" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="F38" s="59">
+      <c r="D38" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="F38" s="51">
         <v>20</v>
       </c>
-      <c r="G38" s="59">
-        <v>0</v>
-      </c>
-      <c r="H38" s="59">
-        <v>1.7103412922069461E-7</v>
-      </c>
-      <c r="I38" s="59">
-        <v>9.5788970955973505E-7</v>
-      </c>
-      <c r="J38" s="59">
-        <v>-2.266782663477714E-7</v>
-      </c>
-      <c r="K38" s="59">
-        <v>9.3302480251823527E-7</v>
-      </c>
-      <c r="L38" s="59">
-        <v>20.240521175283789</v>
-      </c>
-      <c r="M38" s="59">
-        <v>107.9886010336417</v>
-      </c>
-      <c r="N38" s="59" t="s">
+      <c r="G38" s="51">
+        <v>1</v>
+      </c>
+      <c r="H38" s="52">
+        <v>1.0000034004439251</v>
+      </c>
+      <c r="I38" s="52">
+        <v>1.1184213772461109E-5</v>
+      </c>
+      <c r="J38" s="51">
+        <v>-3.6803975193013112E-6</v>
+      </c>
+      <c r="K38" s="51">
+        <v>1.3891659195575229E-5</v>
+      </c>
+      <c r="L38" s="51">
+        <v>20.479643918171281</v>
+      </c>
+      <c r="M38" s="51">
+        <v>108.00508197528789</v>
+      </c>
+      <c r="N38" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="O38" s="59" t="s">
+      <c r="O38" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="P38" s="59">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="59">
-        <v>0</v>
-      </c>
-      <c r="R38" s="59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="59" t="s">
+      <c r="P38" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="51">
+        <v>0</v>
+      </c>
+      <c r="R38" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="B39" s="59">
+      <c r="B39" s="51">
         <v>1000000</v>
       </c>
-      <c r="C39" s="59">
+      <c r="C39" s="51">
         <v>1000000</v>
       </c>
-      <c r="D39" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="E39" s="59" t="s">
-        <v>116</v>
-      </c>
-      <c r="F39" s="59">
+      <c r="D39" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="F39" s="51">
         <v>20</v>
       </c>
-      <c r="G39" s="59">
-        <v>-10</v>
-      </c>
-      <c r="H39" s="59">
-        <v>-9.9999834942891539</v>
-      </c>
-      <c r="I39" s="59">
-        <v>1.2320730914531681E-4</v>
-      </c>
-      <c r="J39" s="59">
-        <v>9.9999877682991176</v>
-      </c>
-      <c r="K39" s="59">
-        <v>9.7928056242306441E-5</v>
-      </c>
-      <c r="L39" s="59">
-        <v>20.59988516004551</v>
-      </c>
-      <c r="M39" s="59">
-        <v>108.0154528224397</v>
-      </c>
-      <c r="N39" s="59" t="s">
+      <c r="G39" s="51">
+        <v>0</v>
+      </c>
+      <c r="H39" s="52">
+        <v>-9.6236139540002298E-9</v>
+      </c>
+      <c r="I39" s="52">
+        <v>1.027462984734989E-6</v>
+      </c>
+      <c r="J39" s="51">
+        <v>-7.6384269314035401E-8</v>
+      </c>
+      <c r="K39" s="51">
+        <v>6.5017047333985786E-7</v>
+      </c>
+      <c r="L39" s="51">
+        <v>20.63494115251099</v>
+      </c>
+      <c r="M39" s="51">
+        <v>108.0058471423382</v>
+      </c>
+      <c r="N39" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="O39" s="59" t="s">
+      <c r="O39" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="P39" s="59">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="59">
-        <v>0</v>
-      </c>
-      <c r="R39" s="59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P39" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="51">
+        <v>0</v>
+      </c>
+      <c r="R39" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="59" t="s">
         <v>98</v>
       </c>
@@ -4726,31 +4622,31 @@
         <v>62</v>
       </c>
       <c r="E40" s="59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F40" s="59">
         <v>20</v>
       </c>
       <c r="G40" s="59">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H40" s="59">
-        <v>9.9999867016247457</v>
+        <v>1.7103412922069461E-7</v>
       </c>
       <c r="I40" s="59">
-        <v>7.9946396573448312E-5</v>
+        <v>9.5788970955973505E-7</v>
       </c>
       <c r="J40" s="59">
-        <v>-9.999960350082322</v>
+        <v>-2.266782663477714E-7</v>
       </c>
       <c r="K40" s="59">
-        <v>9.721591329184521E-5</v>
+        <v>9.3302480251823527E-7</v>
       </c>
       <c r="L40" s="59">
-        <v>20.35674483471135</v>
+        <v>20.240521175283789</v>
       </c>
       <c r="M40" s="59">
-        <v>108.0111052243014</v>
+        <v>107.9886010336417</v>
       </c>
       <c r="N40" s="59" t="s">
         <v>64</v>
@@ -4768,7 +4664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="59" t="s">
         <v>98</v>
       </c>
@@ -4782,31 +4678,31 @@
         <v>62</v>
       </c>
       <c r="E41" s="59" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F41" s="59">
         <v>20</v>
       </c>
       <c r="G41" s="59">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="H41" s="59">
-        <v>-3.9791142967976958E-8</v>
+        <v>-9.9999834942891539</v>
       </c>
       <c r="I41" s="59">
-        <v>7.9635580322720186E-7</v>
+        <v>1.2320730914531681E-4</v>
       </c>
       <c r="J41" s="59">
-        <v>3.6935355802024509E-7</v>
+        <v>9.9999877682991176</v>
       </c>
       <c r="K41" s="59">
-        <v>1.1927738504711901E-6</v>
+        <v>9.7928056242306441E-5</v>
       </c>
       <c r="L41" s="59">
-        <v>20.5641937296066</v>
+        <v>20.59988516004551</v>
       </c>
       <c r="M41" s="59">
-        <v>107.9833222306321</v>
+        <v>108.0154528224397</v>
       </c>
       <c r="N41" s="59" t="s">
         <v>64</v>
@@ -4824,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="59" t="s">
         <v>98</v>
       </c>
@@ -4835,34 +4731,34 @@
         <v>1000000</v>
       </c>
       <c r="D42" s="59" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E42" s="59" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F42" s="59">
         <v>20</v>
       </c>
       <c r="G42" s="59">
-        <v>0</v>
-      </c>
-      <c r="H42" s="60">
-        <v>-1.697231747339152E-7</v>
-      </c>
-      <c r="I42" s="60">
-        <v>1.1707008468467739E-6</v>
+        <v>10</v>
+      </c>
+      <c r="H42" s="59">
+        <v>9.9999867016247457</v>
+      </c>
+      <c r="I42" s="59">
+        <v>7.9946396573448312E-5</v>
       </c>
       <c r="J42" s="59">
-        <v>3.1999798081163638E-7</v>
+        <v>-9.999960350082322</v>
       </c>
       <c r="K42" s="59">
-        <v>1.2943151240888489E-6</v>
+        <v>9.721591329184521E-5</v>
       </c>
       <c r="L42" s="59">
-        <v>20.186462906793189</v>
+        <v>20.35674483471135</v>
       </c>
       <c r="M42" s="59">
-        <v>108.0052172496104</v>
+        <v>108.0111052243014</v>
       </c>
       <c r="N42" s="59" t="s">
         <v>64</v>
@@ -4880,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="59" t="s">
         <v>98</v>
       </c>
@@ -4891,34 +4787,34 @@
         <v>1000000</v>
       </c>
       <c r="D43" s="59" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E43" s="59" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F43" s="59">
         <v>20</v>
       </c>
       <c r="G43" s="59">
-        <v>-10</v>
-      </c>
-      <c r="H43" s="60">
-        <v>-9.9999897520679237</v>
-      </c>
-      <c r="I43" s="60">
-        <v>1.217751345413785E-4</v>
+        <v>0</v>
+      </c>
+      <c r="H43" s="59">
+        <v>-3.9791142967976958E-8</v>
+      </c>
+      <c r="I43" s="59">
+        <v>7.9635580322720186E-7</v>
       </c>
       <c r="J43" s="59">
-        <v>-1.032282241689853E-5</v>
+        <v>3.6935355802024509E-7</v>
       </c>
       <c r="K43" s="59">
-        <v>1.0305123698720179E-4</v>
+        <v>1.1927738504711901E-6</v>
       </c>
       <c r="L43" s="59">
-        <v>20.557524970049279</v>
+        <v>20.5641937296066</v>
       </c>
       <c r="M43" s="59">
-        <v>108.00404310341629</v>
+        <v>107.9833222306321</v>
       </c>
       <c r="N43" s="59" t="s">
         <v>64</v>
@@ -4936,7 +4832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="59" t="s">
         <v>98</v>
       </c>
@@ -4950,31 +4846,31 @@
         <v>77</v>
       </c>
       <c r="E44" s="59" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F44" s="59">
         <v>20</v>
       </c>
       <c r="G44" s="59">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H44" s="60">
-        <v>9.9999698150890044</v>
+        <v>-1.697231747339152E-7</v>
       </c>
       <c r="I44" s="60">
-        <v>8.1064554471068907E-5</v>
+        <v>1.1707008468467739E-6</v>
       </c>
       <c r="J44" s="59">
-        <v>3.183769613441527E-5</v>
+        <v>3.1999798081163638E-7</v>
       </c>
       <c r="K44" s="59">
-        <v>8.750071707608403E-5</v>
+        <v>1.2943151240888489E-6</v>
       </c>
       <c r="L44" s="59">
-        <v>20.432099374045091</v>
+        <v>20.186462906793189</v>
       </c>
       <c r="M44" s="59">
-        <v>107.9791366768105</v>
+        <v>108.0052172496104</v>
       </c>
       <c r="N44" s="59" t="s">
         <v>64</v>
@@ -4992,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="59" t="s">
         <v>98</v>
       </c>
@@ -5006,31 +4902,31 @@
         <v>77</v>
       </c>
       <c r="E45" s="59" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F45" s="59">
         <v>20</v>
       </c>
       <c r="G45" s="59">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="H45" s="60">
-        <v>9.1739954203842216E-8</v>
+        <v>-9.9999897520679237</v>
       </c>
       <c r="I45" s="60">
-        <v>1.018800988611917E-6</v>
+        <v>1.217751345413785E-4</v>
       </c>
       <c r="J45" s="59">
-        <v>-1.7634512055898261E-7</v>
+        <v>-1.032282241689853E-5</v>
       </c>
       <c r="K45" s="59">
-        <v>9.5729797521453914E-7</v>
+        <v>1.0305123698720179E-4</v>
       </c>
       <c r="L45" s="59">
-        <v>20.750685836900029</v>
+        <v>20.557524970049279</v>
       </c>
       <c r="M45" s="59">
-        <v>107.9802135232455</v>
+        <v>108.00404310341629</v>
       </c>
       <c r="N45" s="59" t="s">
         <v>64</v>
@@ -5048,198 +4944,186 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="61" t="s">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="59">
+        <v>1000000</v>
+      </c>
+      <c r="C46" s="59">
+        <v>1000000</v>
+      </c>
+      <c r="D46" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="59" t="s">
+        <v>121</v>
+      </c>
+      <c r="F46" s="59">
+        <v>20</v>
+      </c>
+      <c r="G46" s="59">
+        <v>10</v>
+      </c>
+      <c r="H46" s="60">
+        <v>9.9999698150890044</v>
+      </c>
+      <c r="I46" s="60">
+        <v>8.1064554471068907E-5</v>
+      </c>
+      <c r="J46" s="59">
+        <v>3.183769613441527E-5</v>
+      </c>
+      <c r="K46" s="59">
+        <v>8.750071707608403E-5</v>
+      </c>
+      <c r="L46" s="59">
+        <v>20.432099374045091</v>
+      </c>
+      <c r="M46" s="59">
+        <v>107.9791366768105</v>
+      </c>
+      <c r="N46" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="O46" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="P46" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="59">
+        <v>0</v>
+      </c>
+      <c r="R46" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="59">
+        <v>1000000</v>
+      </c>
+      <c r="C47" s="59">
+        <v>1000000</v>
+      </c>
+      <c r="D47" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="F47" s="59">
+        <v>20</v>
+      </c>
+      <c r="G47" s="59">
+        <v>0</v>
+      </c>
+      <c r="H47" s="60">
+        <v>9.1739954203842216E-8</v>
+      </c>
+      <c r="I47" s="60">
+        <v>1.018800988611917E-6</v>
+      </c>
+      <c r="J47" s="59">
+        <v>-1.7634512055898261E-7</v>
+      </c>
+      <c r="K47" s="59">
+        <v>9.5729797521453914E-7</v>
+      </c>
+      <c r="L47" s="59">
+        <v>20.750685836900029</v>
+      </c>
+      <c r="M47" s="59">
+        <v>107.9802135232455</v>
+      </c>
+      <c r="N47" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="O47" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="P47" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="59">
+        <v>0</v>
+      </c>
+      <c r="R47" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="61" t="s">
+      <c r="B49" s="61" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="E48" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="G48" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="H48" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="I48" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="J48" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="K48" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="L48" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="M48" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="N48" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="O48" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="P48" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q48" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="R48" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="S48" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="T48" s="42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A49" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="B49" s="42">
-        <v>100000000</v>
-      </c>
-      <c r="C49" s="42">
-        <v>10000000</v>
-      </c>
-      <c r="D49" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="E49" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="F49" s="42">
-        <v>20</v>
-      </c>
-      <c r="G49" s="42">
-        <v>0</v>
-      </c>
-      <c r="H49" s="42">
-        <v>-3.571497444227242E-7</v>
-      </c>
-      <c r="I49" s="42">
-        <v>1.097101390673675E-6</v>
-      </c>
-      <c r="J49" s="42">
-        <v>1.101983103055069E-7</v>
-      </c>
-      <c r="K49" s="42">
-        <v>1.009974129675528E-6</v>
-      </c>
-      <c r="L49" s="42">
-        <v>20.620695737635199</v>
-      </c>
-      <c r="M49" s="42">
-        <v>107.99774652189549</v>
-      </c>
-      <c r="N49" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="O49" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="P49" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="42">
-        <v>0</v>
-      </c>
-      <c r="R49" s="42">
-        <v>0</v>
-      </c>
-      <c r="S49" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="T49" s="63" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="B50" s="42">
-        <v>100000000</v>
-      </c>
-      <c r="C50" s="42">
-        <v>10000000</v>
+        <v>42</v>
+      </c>
+      <c r="B50" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>44</v>
       </c>
       <c r="D50" s="42" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E50" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="F50" s="42">
-        <v>20</v>
-      </c>
-      <c r="G50" s="42">
-        <v>-0.1</v>
-      </c>
-      <c r="H50" s="42">
-        <v>-9.9999587784921906E-2</v>
-      </c>
-      <c r="I50" s="42">
-        <v>2.23798238765592E-6</v>
-      </c>
-      <c r="J50" s="42">
-        <v>1.000020765938491E-2</v>
-      </c>
-      <c r="K50" s="42">
-        <v>9.5632950185285167E-7</v>
-      </c>
-      <c r="L50" s="42">
-        <v>20.59055602989547</v>
-      </c>
-      <c r="M50" s="42">
-        <v>108.01473032805541</v>
+        <v>46</v>
+      </c>
+      <c r="F50" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="G50" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="H50" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="I50" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="J50" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="K50" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="L50" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="M50" s="42" t="s">
+        <v>53</v>
       </c>
       <c r="N50" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="O50" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="P50" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="42">
-        <v>0</v>
-      </c>
-      <c r="R50" s="42">
-        <v>0</v>
-      </c>
-      <c r="S50" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="T50" s="65" t="s">
-        <v>70</v>
+        <v>55</v>
+      </c>
+      <c r="P50" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q50" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="R50" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="S50" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="T50" s="42" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
@@ -5256,31 +5140,31 @@
         <v>62</v>
       </c>
       <c r="E51" s="42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F51" s="42">
         <v>20</v>
       </c>
       <c r="G51" s="42">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H51" s="42">
-        <v>9.9999264653670511E-2</v>
+        <v>-3.571497444227242E-7</v>
       </c>
       <c r="I51" s="42">
-        <v>1.335161239397657E-6</v>
+        <v>1.097101390673675E-6</v>
       </c>
       <c r="J51" s="42">
-        <v>-9.9998122319977477E-3</v>
+        <v>1.101983103055069E-7</v>
       </c>
       <c r="K51" s="42">
-        <v>1.157519919180399E-6</v>
+        <v>1.009974129675528E-6</v>
       </c>
       <c r="L51" s="42">
-        <v>20.633736963166061</v>
+        <v>20.620695737635199</v>
       </c>
       <c r="M51" s="42">
-        <v>108.0017629344367</v>
+        <v>107.99774652189549</v>
       </c>
       <c r="N51" s="42" t="s">
         <v>64</v>
@@ -5297,11 +5181,11 @@
       <c r="R51" s="42">
         <v>0</v>
       </c>
-      <c r="S51" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="T51" s="65" t="s">
-        <v>73</v>
+      <c r="S51" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="T51" s="63" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
@@ -5318,31 +5202,31 @@
         <v>62</v>
       </c>
       <c r="E52" s="42" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F52" s="42">
         <v>20</v>
       </c>
       <c r="G52" s="42">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="H52" s="42">
-        <v>1.7078281539309991E-7</v>
+        <v>-9.9999587784921906E-2</v>
       </c>
       <c r="I52" s="42">
-        <v>1.1005327988159939E-6</v>
+        <v>2.23798238765592E-6</v>
       </c>
       <c r="J52" s="42">
-        <v>-2.7071424382348861E-7</v>
+        <v>1.000020765938491E-2</v>
       </c>
       <c r="K52" s="42">
-        <v>1.123348877359649E-6</v>
+        <v>9.5632950185285167E-7</v>
       </c>
       <c r="L52" s="42">
-        <v>20.622763154196051</v>
+        <v>20.59055602989547</v>
       </c>
       <c r="M52" s="42">
-        <v>107.99633331319789</v>
+        <v>108.01473032805541</v>
       </c>
       <c r="N52" s="42" t="s">
         <v>64</v>
@@ -5360,10 +5244,10 @@
         <v>0</v>
       </c>
       <c r="S52" s="64" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="T52" s="65" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
@@ -5377,34 +5261,34 @@
         <v>10000000</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E53" s="42" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F53" s="42">
         <v>20</v>
       </c>
       <c r="G53" s="42">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H53" s="42">
-        <v>1.8911951727158461E-7</v>
+        <v>9.9999264653670511E-2</v>
       </c>
       <c r="I53" s="42">
-        <v>1.0869104445720209E-6</v>
+        <v>1.335161239397657E-6</v>
       </c>
       <c r="J53" s="42">
-        <v>-1.054726596527278E-7</v>
+        <v>-9.9998122319977477E-3</v>
       </c>
       <c r="K53" s="42">
-        <v>9.011580739629565E-7</v>
+        <v>1.157519919180399E-6</v>
       </c>
       <c r="L53" s="42">
-        <v>20.599946280508679</v>
+        <v>20.633736963166061</v>
       </c>
       <c r="M53" s="42">
-        <v>108.0096105434848</v>
+        <v>108.0017629344367</v>
       </c>
       <c r="N53" s="42" t="s">
         <v>64</v>
@@ -5422,10 +5306,10 @@
         <v>0</v>
       </c>
       <c r="S53" s="64" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="T53" s="65" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
@@ -5439,34 +5323,34 @@
         <v>10000000</v>
       </c>
       <c r="D54" s="42" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E54" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F54" s="42">
         <v>20</v>
       </c>
       <c r="G54" s="42">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="H54" s="42">
-        <v>-9.9999805686051643E-2</v>
+        <v>1.7078281539309991E-7</v>
       </c>
       <c r="I54" s="42">
-        <v>2.1115933145681151E-6</v>
+        <v>1.1005327988159939E-6</v>
       </c>
       <c r="J54" s="42">
-        <v>-2.1913311786864691E-7</v>
+        <v>-2.7071424382348861E-7</v>
       </c>
       <c r="K54" s="42">
-        <v>1.1272967532656981E-6</v>
+        <v>1.123348877359649E-6</v>
       </c>
       <c r="L54" s="42">
-        <v>20.1734868927837</v>
+        <v>20.622763154196051</v>
       </c>
       <c r="M54" s="42">
-        <v>108.010575758313</v>
+        <v>107.99633331319789</v>
       </c>
       <c r="N54" s="42" t="s">
         <v>64</v>
@@ -5484,10 +5368,10 @@
         <v>0</v>
       </c>
       <c r="S54" s="64" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="T54" s="65" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
@@ -5504,31 +5388,31 @@
         <v>77</v>
       </c>
       <c r="E55" s="42" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F55" s="42">
         <v>20</v>
       </c>
       <c r="G55" s="42">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H55" s="42">
-        <v>0.1000001765880036</v>
+        <v>1.8911951727158461E-7</v>
       </c>
       <c r="I55" s="42">
-        <v>1.7240729489488951E-6</v>
+        <v>1.0869104445720209E-6</v>
       </c>
       <c r="J55" s="42">
-        <v>-2.891694682635999E-7</v>
+        <v>-1.054726596527278E-7</v>
       </c>
       <c r="K55" s="42">
-        <v>1.119342691841005E-6</v>
+        <v>9.011580739629565E-7</v>
       </c>
       <c r="L55" s="42">
-        <v>20.307982799432271</v>
+        <v>20.599946280508679</v>
       </c>
       <c r="M55" s="42">
-        <v>107.9930375009486</v>
+        <v>108.0096105434848</v>
       </c>
       <c r="N55" s="42" t="s">
         <v>64</v>
@@ -5545,11 +5429,11 @@
       <c r="R55" s="42">
         <v>0</v>
       </c>
-      <c r="S55" s="66" t="s">
-        <v>85</v>
-      </c>
-      <c r="T55" s="67" t="s">
-        <v>86</v>
+      <c r="S55" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="T55" s="65" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
@@ -5566,31 +5450,31 @@
         <v>77</v>
       </c>
       <c r="E56" s="42" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F56" s="42">
         <v>20</v>
       </c>
       <c r="G56" s="42">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="H56" s="42">
-        <v>8.3810862204933571E-8</v>
+        <v>-9.9999805686051643E-2</v>
       </c>
       <c r="I56" s="42">
-        <v>8.3501485482641314E-7</v>
+        <v>2.1115933145681151E-6</v>
       </c>
       <c r="J56" s="42">
-        <v>6.0506692722657893E-8</v>
+        <v>-2.1913311786864691E-7</v>
       </c>
       <c r="K56" s="42">
-        <v>9.9853133312348311E-7</v>
+        <v>1.1272967532656981E-6</v>
       </c>
       <c r="L56" s="42">
-        <v>20.239389017943061</v>
+        <v>20.1734868927837</v>
       </c>
       <c r="M56" s="42">
-        <v>108.009667149153</v>
+        <v>108.010575758313</v>
       </c>
       <c r="N56" s="42" t="s">
         <v>64</v>
@@ -5606,6 +5490,12 @@
       </c>
       <c r="R56" s="42">
         <v>0</v>
+      </c>
+      <c r="S56" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="T56" s="65" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
@@ -5619,34 +5509,34 @@
         <v>10000000</v>
       </c>
       <c r="D57" s="42" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="E57" s="42" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F57" s="42">
         <v>20</v>
       </c>
       <c r="G57" s="42">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H57" s="42">
-        <v>-8.3892529561174833E-8</v>
+        <v>0.1000001765880036</v>
       </c>
       <c r="I57" s="42">
-        <v>1.129741672908929E-6</v>
+        <v>1.7240729489488951E-6</v>
       </c>
       <c r="J57" s="42">
-        <v>3.2659315810514668E-7</v>
+        <v>-2.891694682635999E-7</v>
       </c>
       <c r="K57" s="42">
-        <v>1.158124753683184E-6</v>
+        <v>1.119342691841005E-6</v>
       </c>
       <c r="L57" s="42">
-        <v>20.58955897737513</v>
+        <v>20.307982799432271</v>
       </c>
       <c r="M57" s="42">
-        <v>108.01080176389139</v>
+        <v>107.9930375009486</v>
       </c>
       <c r="N57" s="42" t="s">
         <v>64</v>
@@ -5662,6 +5552,12 @@
       </c>
       <c r="R57" s="42">
         <v>0</v>
+      </c>
+      <c r="S57" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="T57" s="67" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
@@ -5675,34 +5571,34 @@
         <v>10000000</v>
       </c>
       <c r="D58" s="42" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="E58" s="42" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F58" s="42">
         <v>20</v>
       </c>
       <c r="G58" s="42">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H58" s="42">
-        <v>-1.000002406615095</v>
+        <v>8.3810862204933571E-8</v>
       </c>
       <c r="I58" s="42">
-        <v>1.007848227596929E-5</v>
+        <v>8.3501485482641314E-7</v>
       </c>
       <c r="J58" s="42">
-        <v>9.9998578676185626E-2</v>
+        <v>6.0506692722657893E-8</v>
       </c>
       <c r="K58" s="42">
-        <v>2.055513454956669E-6</v>
+        <v>9.9853133312348311E-7</v>
       </c>
       <c r="L58" s="42">
-        <v>20.556507992158782</v>
+        <v>20.239389017943061</v>
       </c>
       <c r="M58" s="42">
-        <v>108.0097313982079</v>
+        <v>108.009667149153</v>
       </c>
       <c r="N58" s="42" t="s">
         <v>64</v>
@@ -5734,31 +5630,31 @@
         <v>62</v>
       </c>
       <c r="E59" s="42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F59" s="42">
         <v>20</v>
       </c>
       <c r="G59" s="42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59" s="42">
-        <v>0.9999996665834251</v>
+        <v>-8.3892529561174833E-8</v>
       </c>
       <c r="I59" s="42">
-        <v>1.024608554929067E-5</v>
+        <v>1.129741672908929E-6</v>
       </c>
       <c r="J59" s="42">
-        <v>-9.9999750454204783E-2</v>
+        <v>3.2659315810514668E-7</v>
       </c>
       <c r="K59" s="42">
-        <v>2.1492891208987191E-6</v>
+        <v>1.158124753683184E-6</v>
       </c>
       <c r="L59" s="42">
-        <v>20.664371084027341</v>
+        <v>20.58955897737513</v>
       </c>
       <c r="M59" s="42">
-        <v>108.0091635299481</v>
+        <v>108.01080176389139</v>
       </c>
       <c r="N59" s="42" t="s">
         <v>64</v>
@@ -5790,31 +5686,31 @@
         <v>62</v>
       </c>
       <c r="E60" s="42" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F60" s="42">
         <v>20</v>
       </c>
       <c r="G60" s="42">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H60" s="42">
-        <v>1.4318234606517781E-7</v>
+        <v>-1.000002406615095</v>
       </c>
       <c r="I60" s="42">
-        <v>8.1917274029067167E-7</v>
+        <v>1.007848227596929E-5</v>
       </c>
       <c r="J60" s="42">
-        <v>-3.9739597528511632E-8</v>
+        <v>9.9998578676185626E-2</v>
       </c>
       <c r="K60" s="42">
-        <v>7.9253345396706868E-7</v>
+        <v>2.055513454956669E-6</v>
       </c>
       <c r="L60" s="42">
-        <v>20.397244939444199</v>
+        <v>20.556507992158782</v>
       </c>
       <c r="M60" s="42">
-        <v>107.9778252335468</v>
+        <v>108.0097313982079</v>
       </c>
       <c r="N60" s="42" t="s">
         <v>64</v>
@@ -5843,34 +5739,34 @@
         <v>10000000</v>
       </c>
       <c r="D61" s="42" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E61" s="42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F61" s="42">
         <v>20</v>
       </c>
       <c r="G61" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" s="42">
-        <v>1.9190815592624419E-7</v>
+        <v>0.9999996665834251</v>
       </c>
       <c r="I61" s="42">
-        <v>1.1314651682880089E-6</v>
+        <v>1.024608554929067E-5</v>
       </c>
       <c r="J61" s="42">
-        <v>4.4357970087597112E-7</v>
+        <v>-9.9999750454204783E-2</v>
       </c>
       <c r="K61" s="42">
-        <v>9.3620917524069772E-7</v>
+        <v>2.1492891208987191E-6</v>
       </c>
       <c r="L61" s="42">
-        <v>20.3956404061421</v>
+        <v>20.664371084027341</v>
       </c>
       <c r="M61" s="42">
-        <v>107.973989332239</v>
+        <v>108.0091635299481</v>
       </c>
       <c r="N61" s="42" t="s">
         <v>64</v>
@@ -5899,34 +5795,34 @@
         <v>10000000</v>
       </c>
       <c r="D62" s="42" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E62" s="42" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F62" s="42">
         <v>20</v>
       </c>
       <c r="G62" s="42">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H62" s="42">
-        <v>-1.0000022115059251</v>
+        <v>1.4318234606517781E-7</v>
       </c>
       <c r="I62" s="42">
-        <v>1.004776018512994E-5</v>
+        <v>8.1917274029067167E-7</v>
       </c>
       <c r="J62" s="42">
-        <v>-5.5183336622669574E-7</v>
+        <v>-3.9739597528511632E-8</v>
       </c>
       <c r="K62" s="42">
-        <v>2.1611713918934502E-6</v>
+        <v>7.9253345396706868E-7</v>
       </c>
       <c r="L62" s="42">
-        <v>20.38971364283724</v>
+        <v>20.397244939444199</v>
       </c>
       <c r="M62" s="42">
-        <v>107.9990377412054</v>
+        <v>107.9778252335468</v>
       </c>
       <c r="N62" s="42" t="s">
         <v>64</v>
@@ -5958,31 +5854,31 @@
         <v>77</v>
       </c>
       <c r="E63" s="42" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F63" s="42">
         <v>20</v>
       </c>
       <c r="G63" s="42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63" s="42">
-        <v>0.99999866530618742</v>
+        <v>1.9190815592624419E-7</v>
       </c>
       <c r="I63" s="42">
-        <v>1.065423223615718E-5</v>
+        <v>1.1314651682880089E-6</v>
       </c>
       <c r="J63" s="42">
-        <v>-5.4923730617626944E-7</v>
+        <v>4.4357970087597112E-7</v>
       </c>
       <c r="K63" s="42">
-        <v>1.769267262190784E-6</v>
+        <v>9.3620917524069772E-7</v>
       </c>
       <c r="L63" s="42">
-        <v>20.483279693783839</v>
+        <v>20.3956404061421</v>
       </c>
       <c r="M63" s="42">
-        <v>108.0063751941386</v>
+        <v>107.973989332239</v>
       </c>
       <c r="N63" s="42" t="s">
         <v>64</v>
@@ -6014,31 +5910,31 @@
         <v>77</v>
       </c>
       <c r="E64" s="42" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F64" s="42">
         <v>20</v>
       </c>
       <c r="G64" s="42">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H64" s="42">
-        <v>1.368440872449583E-7</v>
+        <v>-1.0000022115059251</v>
       </c>
       <c r="I64" s="42">
-        <v>7.9141281867660523E-7</v>
+        <v>1.004776018512994E-5</v>
       </c>
       <c r="J64" s="42">
-        <v>1.2887184826873221E-7</v>
+        <v>-5.5183336622669574E-7</v>
       </c>
       <c r="K64" s="42">
-        <v>1.195967093536109E-6</v>
+        <v>2.1611713918934502E-6</v>
       </c>
       <c r="L64" s="42">
-        <v>20.547149068885609</v>
+        <v>20.38971364283724</v>
       </c>
       <c r="M64" s="42">
-        <v>108.00795049079061</v>
+        <v>107.9990377412054</v>
       </c>
       <c r="N64" s="42" t="s">
         <v>64</v>
@@ -6067,34 +5963,34 @@
         <v>10000000</v>
       </c>
       <c r="D65" s="42" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="E65" s="42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F65" s="42">
         <v>20</v>
       </c>
       <c r="G65" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" s="42">
-        <v>-2.231080179554421E-7</v>
+        <v>0.99999866530618742</v>
       </c>
       <c r="I65" s="42">
-        <v>9.1652434399653769E-7</v>
+        <v>1.065423223615718E-5</v>
       </c>
       <c r="J65" s="42">
-        <v>-7.1000345332782564E-8</v>
+        <v>-5.4923730617626944E-7</v>
       </c>
       <c r="K65" s="42">
-        <v>9.1055606767222927E-7</v>
+        <v>1.769267262190784E-6</v>
       </c>
       <c r="L65" s="42">
-        <v>20.56802957637986</v>
+        <v>20.483279693783839</v>
       </c>
       <c r="M65" s="42">
-        <v>107.9994706080209</v>
+        <v>108.0063751941386</v>
       </c>
       <c r="N65" s="42" t="s">
         <v>64</v>
@@ -6123,34 +6019,34 @@
         <v>10000000</v>
       </c>
       <c r="D66" s="42" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="E66" s="42" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F66" s="42">
         <v>20</v>
       </c>
       <c r="G66" s="42">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="H66" s="42">
-        <v>-10.00002185654624</v>
+        <v>1.368440872449583E-7</v>
       </c>
       <c r="I66" s="42">
-        <v>1.020294024796482E-4</v>
+        <v>7.9141281867660523E-7</v>
       </c>
       <c r="J66" s="42">
-        <v>1.0000002630139899</v>
+        <v>1.2887184826873221E-7</v>
       </c>
       <c r="K66" s="42">
-        <v>1.042839523377521E-5</v>
+        <v>1.195967093536109E-6</v>
       </c>
       <c r="L66" s="42">
-        <v>20.667390910289491</v>
+        <v>20.547149068885609</v>
       </c>
       <c r="M66" s="42">
-        <v>107.9892742646004</v>
+        <v>108.00795049079061</v>
       </c>
       <c r="N66" s="42" t="s">
         <v>64</v>
@@ -6182,31 +6078,31 @@
         <v>62</v>
       </c>
       <c r="E67" s="42" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F67" s="42">
         <v>20</v>
       </c>
       <c r="G67" s="42">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H67" s="42">
-        <v>10.00002445846477</v>
+        <v>-2.231080179554421E-7</v>
       </c>
       <c r="I67" s="42">
-        <v>1.038073553014757E-4</v>
+        <v>9.1652434399653769E-7</v>
       </c>
       <c r="J67" s="42">
-        <v>-1.0000016969210741</v>
+        <v>-7.1000345332782564E-8</v>
       </c>
       <c r="K67" s="42">
-        <v>1.291755544239828E-5</v>
+        <v>9.1055606767222927E-7</v>
       </c>
       <c r="L67" s="42">
-        <v>20.61625005268829</v>
+        <v>20.56802957637986</v>
       </c>
       <c r="M67" s="42">
-        <v>108.02754481667201</v>
+        <v>107.9994706080209</v>
       </c>
       <c r="N67" s="42" t="s">
         <v>64</v>
@@ -6238,31 +6134,31 @@
         <v>62</v>
       </c>
       <c r="E68" s="42" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F68" s="42">
         <v>20</v>
       </c>
       <c r="G68" s="42">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="H68" s="42">
-        <v>7.8263282877592342E-8</v>
+        <v>-10.00002185654624</v>
       </c>
       <c r="I68" s="42">
-        <v>9.6847749438324071E-7</v>
+        <v>1.020294024796482E-4</v>
       </c>
       <c r="J68" s="42">
-        <v>5.0454902356203246E-7</v>
+        <v>1.0000002630139899</v>
       </c>
       <c r="K68" s="42">
-        <v>7.3371960451695662E-7</v>
+        <v>1.042839523377521E-5</v>
       </c>
       <c r="L68" s="42">
-        <v>20.737059337043721</v>
+        <v>20.667390910289491</v>
       </c>
       <c r="M68" s="42">
-        <v>108.0035577910669</v>
+        <v>107.9892742646004</v>
       </c>
       <c r="N68" s="42" t="s">
         <v>64</v>
@@ -6291,34 +6187,34 @@
         <v>10000000</v>
       </c>
       <c r="D69" s="42" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E69" s="42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F69" s="42">
         <v>20</v>
       </c>
       <c r="G69" s="42">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H69" s="42">
-        <v>-1.252397540317582E-8</v>
+        <v>10.00002445846477</v>
       </c>
       <c r="I69" s="42">
-        <v>1.0814580927887251E-6</v>
+        <v>1.038073553014757E-4</v>
       </c>
       <c r="J69" s="42">
-        <v>4.4235771280743362E-8</v>
+        <v>-1.0000016969210741</v>
       </c>
       <c r="K69" s="42">
-        <v>1.050471117362541E-6</v>
+        <v>1.291755544239828E-5</v>
       </c>
       <c r="L69" s="42">
-        <v>20.79034154899734</v>
+        <v>20.61625005268829</v>
       </c>
       <c r="M69" s="42">
-        <v>108.00509893987611</v>
+        <v>108.02754481667201</v>
       </c>
       <c r="N69" s="42" t="s">
         <v>64</v>
@@ -6347,34 +6243,34 @@
         <v>10000000</v>
       </c>
       <c r="D70" s="42" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E70" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F70" s="42">
         <v>20</v>
       </c>
       <c r="G70" s="42">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="H70" s="42">
-        <v>-10.000008394823</v>
+        <v>7.8263282877592342E-8</v>
       </c>
       <c r="I70" s="42">
-        <v>1.032306410477313E-4</v>
+        <v>9.6847749438324071E-7</v>
       </c>
       <c r="J70" s="42">
-        <v>3.7850573156504889E-6</v>
+        <v>5.0454902356203246E-7</v>
       </c>
       <c r="K70" s="42">
-        <v>1.144909367316122E-5</v>
+        <v>7.3371960451695662E-7</v>
       </c>
       <c r="L70" s="42">
-        <v>20.67338594692006</v>
+        <v>20.737059337043721</v>
       </c>
       <c r="M70" s="42">
-        <v>108.0121980051719</v>
+        <v>108.0035577910669</v>
       </c>
       <c r="N70" s="42" t="s">
         <v>64</v>
@@ -6406,31 +6302,31 @@
         <v>77</v>
       </c>
       <c r="E71" s="42" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F71" s="42">
         <v>20</v>
       </c>
       <c r="G71" s="42">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H71" s="42">
-        <v>9.9999970890213579</v>
+        <v>-1.252397540317582E-8</v>
       </c>
       <c r="I71" s="42">
-        <v>1.332366099744941E-4</v>
+        <v>1.0814580927887251E-6</v>
       </c>
       <c r="J71" s="42">
-        <v>-2.8196096354298438E-6</v>
+        <v>4.4235771280743362E-8</v>
       </c>
       <c r="K71" s="42">
-        <v>1.193618690547882E-5</v>
+        <v>1.050471117362541E-6</v>
       </c>
       <c r="L71" s="42">
-        <v>20.2470599243719</v>
+        <v>20.79034154899734</v>
       </c>
       <c r="M71" s="42">
-        <v>107.994715078377</v>
+        <v>108.00509893987611</v>
       </c>
       <c r="N71" s="42" t="s">
         <v>64</v>
@@ -6462,31 +6358,31 @@
         <v>77</v>
       </c>
       <c r="E72" s="42" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F72" s="42">
         <v>20</v>
       </c>
       <c r="G72" s="42">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="H72" s="42">
-        <v>-3.6521992892610022E-8</v>
+        <v>-10.000008394823</v>
       </c>
       <c r="I72" s="42">
-        <v>9.1205977498331018E-7</v>
+        <v>1.032306410477313E-4</v>
       </c>
       <c r="J72" s="42">
-        <v>7.2209246987649033E-8</v>
+        <v>3.7850573156504889E-6</v>
       </c>
       <c r="K72" s="42">
-        <v>1.009103663857629E-6</v>
+        <v>1.144909367316122E-5</v>
       </c>
       <c r="L72" s="42">
-        <v>20.394440816923229</v>
+        <v>20.67338594692006</v>
       </c>
       <c r="M72" s="42">
-        <v>107.9963973142941</v>
+        <v>108.0121980051719</v>
       </c>
       <c r="N72" s="42" t="s">
         <v>64</v>
@@ -6504,9 +6400,121 @@
         <v>0</v>
       </c>
     </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B73" s="42">
+        <v>100000000</v>
+      </c>
+      <c r="C73" s="42">
+        <v>10000000</v>
+      </c>
+      <c r="D73" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E73" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="F73" s="42">
+        <v>20</v>
+      </c>
+      <c r="G73" s="42">
+        <v>10</v>
+      </c>
+      <c r="H73" s="42">
+        <v>9.9999970890213579</v>
+      </c>
+      <c r="I73" s="42">
+        <v>1.332366099744941E-4</v>
+      </c>
+      <c r="J73" s="42">
+        <v>-2.8196096354298438E-6</v>
+      </c>
+      <c r="K73" s="42">
+        <v>1.193618690547882E-5</v>
+      </c>
+      <c r="L73" s="42">
+        <v>20.2470599243719</v>
+      </c>
+      <c r="M73" s="42">
+        <v>107.994715078377</v>
+      </c>
+      <c r="N73" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="O73" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="P73" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q73" s="42">
+        <v>0</v>
+      </c>
+      <c r="R73" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B74" s="42">
+        <v>100000000</v>
+      </c>
+      <c r="C74" s="42">
+        <v>10000000</v>
+      </c>
+      <c r="D74" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E74" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="F74" s="42">
+        <v>20</v>
+      </c>
+      <c r="G74" s="42">
+        <v>0</v>
+      </c>
+      <c r="H74" s="42">
+        <v>-3.6521992892610022E-8</v>
+      </c>
+      <c r="I74" s="42">
+        <v>9.1205977498331018E-7</v>
+      </c>
+      <c r="J74" s="42">
+        <v>7.2209246987649033E-8</v>
+      </c>
+      <c r="K74" s="42">
+        <v>1.009103663857629E-6</v>
+      </c>
+      <c r="L74" s="42">
+        <v>20.394440816923229</v>
+      </c>
+      <c r="M74" s="42">
+        <v>107.9963973142941</v>
+      </c>
+      <c r="N74" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="O74" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="P74" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="42">
+        <v>0</v>
+      </c>
+      <c r="R74" s="42">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6514,7 +6522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="540" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
@@ -8693,13 +8701,13 @@
       <c r="J67" s="21" t="s">
         <v>442</v>
       </c>
-      <c r="K67" s="30">
+      <c r="K67" s="27">
         <v>1.000001000001</v>
       </c>
-      <c r="L67" s="31">
+      <c r="L67" s="28">
         <v>1.4142163908044624E-6</v>
       </c>
-      <c r="M67" s="32">
+      <c r="M67" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N67" s="9" t="s">
@@ -8734,13 +8742,13 @@
       <c r="J68" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="K68" s="27">
+      <c r="K68" s="30">
         <v>1.000001000001</v>
       </c>
-      <c r="L68" s="28">
+      <c r="L68" s="31">
         <v>1.414216390804462E-6</v>
       </c>
-      <c r="M68" s="29">
+      <c r="M68" s="32">
         <v>120.87512900978579</v>
       </c>
       <c r="N68" s="14" t="s">
@@ -8775,13 +8783,13 @@
       <c r="J69" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="K69" s="30">
+      <c r="K69" s="27">
         <v>1.0000013000016901</v>
       </c>
-      <c r="L69" s="31">
+      <c r="L69" s="28">
         <v>9.1924120556809292E-7</v>
       </c>
-      <c r="M69" s="32">
+      <c r="M69" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N69" s="9" t="s">
@@ -8816,13 +8824,13 @@
       <c r="J70" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="K70" s="30">
+      <c r="K70" s="27">
         <v>1.00000120000144</v>
       </c>
-      <c r="L70" s="31">
+      <c r="L70" s="28">
         <v>7.0710847824587696E-7</v>
       </c>
-      <c r="M70" s="32">
+      <c r="M70" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N70" s="9" t="s">
@@ -8848,13 +8856,13 @@
       <c r="J71" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="K71" s="30">
+      <c r="K71" s="27">
         <v>1.000001050001103</v>
       </c>
-      <c r="L71" s="31">
+      <c r="L71" s="28">
         <v>8.1317450603009567E-7</v>
       </c>
-      <c r="M71" s="32">
+      <c r="M71" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N71" s="9" t="s">
@@ -8884,13 +8892,13 @@
       <c r="J72" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="K72" s="30">
+      <c r="K72" s="27">
         <v>1.00000120000144</v>
       </c>
-      <c r="L72" s="31">
+      <c r="L72" s="28">
         <v>3.5355423912293848E-7</v>
       </c>
-      <c r="M72" s="32">
+      <c r="M72" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N72" s="9" t="s">
@@ -8925,13 +8933,13 @@
       <c r="J73" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="K73" s="30">
+      <c r="K73" s="27">
         <v>1.0000011500013219</v>
       </c>
-      <c r="L73" s="31">
+      <c r="L73" s="28">
         <v>2.4748794263723231E-7</v>
       </c>
-      <c r="M73" s="32">
+      <c r="M73" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N73" s="9" t="s">
@@ -8966,13 +8974,13 @@
       <c r="J74" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="K74" s="27">
+      <c r="K74" s="30">
         <v>1.000001000001</v>
       </c>
-      <c r="L74" s="28">
+      <c r="L74" s="31">
         <v>8.4852983448267751E-7</v>
       </c>
-      <c r="M74" s="29">
+      <c r="M74" s="32">
         <v>120.87512900978579</v>
       </c>
       <c r="N74" s="14" t="s">
@@ -9007,13 +9015,13 @@
       <c r="J75" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="K75" s="30">
+      <c r="K75" s="27">
         <v>1.00000070000049</v>
       </c>
-      <c r="L75" s="31">
+      <c r="L75" s="28">
         <v>7.0710777113708063E-7</v>
       </c>
-      <c r="M75" s="32">
+      <c r="M75" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N75" s="9" t="s">
@@ -9054,7 +9062,7 @@
       <c r="L76" s="34">
         <v>2.9000000000000002E-8</v>
       </c>
-      <c r="M76" s="32">
+      <c r="M76" s="29">
         <v>18</v>
       </c>
       <c r="N76" s="9" t="s">
@@ -9086,7 +9094,7 @@
       <c r="L77" s="34">
         <v>2.9000000000000002E-8</v>
       </c>
-      <c r="M77" s="32">
+      <c r="M77" s="29">
         <v>18</v>
       </c>
       <c r="N77" s="9" t="s">
@@ -9245,13 +9253,13 @@
       <c r="J86" s="21" t="s">
         <v>442</v>
       </c>
-      <c r="K86" s="30">
+      <c r="K86" s="27">
         <v>1</v>
       </c>
-      <c r="L86" s="31">
+      <c r="L86" s="28">
         <v>1.4142135623730949E-6</v>
       </c>
-      <c r="M86" s="32">
+      <c r="M86" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N86" s="9" t="s">
@@ -9265,13 +9273,13 @@
       <c r="J87" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="K87" s="27">
+      <c r="K87" s="30">
         <v>1</v>
       </c>
-      <c r="L87" s="28">
+      <c r="L87" s="31">
         <v>1.4142135623730949E-6</v>
       </c>
-      <c r="M87" s="29">
+      <c r="M87" s="32">
         <v>120.87512900978579</v>
       </c>
       <c r="N87" s="14" t="s">
@@ -9288,13 +9296,13 @@
       <c r="J88" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="K88" s="30">
+      <c r="K88" s="27">
         <v>1.0000001000000101</v>
       </c>
-      <c r="L88" s="31">
+      <c r="L88" s="28">
         <v>9.1923899939030255E-7</v>
       </c>
-      <c r="M88" s="32">
+      <c r="M88" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N88" s="9" t="s">
@@ -9311,13 +9319,13 @@
       <c r="J89" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="K89" s="30">
+      <c r="K89" s="27">
         <v>1</v>
       </c>
-      <c r="L89" s="31">
+      <c r="L89" s="28">
         <v>7.0710678118654747E-7</v>
       </c>
-      <c r="M89" s="32">
+      <c r="M89" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N89" s="9" t="s">
@@ -9334,13 +9342,13 @@
       <c r="J90" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="K90" s="30">
+      <c r="K90" s="27">
         <v>1.0000000500000019</v>
       </c>
-      <c r="L90" s="31">
+      <c r="L90" s="28">
         <v>8.1317287968181555E-7</v>
       </c>
-      <c r="M90" s="32">
+      <c r="M90" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N90" s="9" t="s">
@@ -9357,13 +9365,13 @@
       <c r="J91" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="K91" s="30">
+      <c r="K91" s="27">
         <v>1.0000002000000401</v>
       </c>
-      <c r="L91" s="31">
+      <c r="L91" s="28">
         <v>3.535535320146725E-7</v>
       </c>
-      <c r="M91" s="32">
+      <c r="M91" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N91" s="9" t="s">
@@ -9380,13 +9388,13 @@
       <c r="J92" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="K92" s="30">
+      <c r="K92" s="27">
         <v>1.0000002000000401</v>
       </c>
-      <c r="L92" s="31">
+      <c r="L92" s="28">
         <v>2.4748747241027072E-7</v>
       </c>
-      <c r="M92" s="32">
+      <c r="M92" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N92" s="9" t="s">
@@ -9403,13 +9411,13 @@
       <c r="J93" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="K93" s="27">
+      <c r="K93" s="30">
         <v>0.99999970000008986</v>
       </c>
-      <c r="L93" s="28">
+      <c r="L93" s="31">
         <v>8.4852762830720346E-7</v>
       </c>
-      <c r="M93" s="29">
+      <c r="M93" s="32">
         <v>120.87512900978579</v>
       </c>
       <c r="N93" s="14" t="s">
@@ -9426,13 +9434,13 @@
       <c r="J94" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="K94" s="30">
+      <c r="K94" s="27">
         <v>0.99999960000015997</v>
       </c>
-      <c r="L94" s="31">
+      <c r="L94" s="28">
         <v>7.07106215501462E-7</v>
       </c>
-      <c r="M94" s="32">
+      <c r="M94" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N94" s="9" t="s">
@@ -9455,7 +9463,7 @@
       <c r="L95" s="34">
         <v>2E-8</v>
       </c>
-      <c r="M95" s="32">
+      <c r="M95" s="29">
         <v>18</v>
       </c>
       <c r="N95" s="9" t="s">
@@ -9478,7 +9486,7 @@
       <c r="L96" s="34">
         <v>2E-8</v>
       </c>
-      <c r="M96" s="32">
+      <c r="M96" s="29">
         <v>18</v>
       </c>
       <c r="N96" s="9" t="s">
@@ -9623,13 +9631,13 @@
       <c r="J105" s="21" t="s">
         <v>442</v>
       </c>
-      <c r="K105" s="30">
+      <c r="K105" s="27">
         <v>1.00000250000625</v>
       </c>
-      <c r="L105" s="31">
+      <c r="L105" s="28">
         <v>1.4142206334674234E-6</v>
       </c>
-      <c r="M105" s="32">
+      <c r="M105" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N105" s="21" t="s">
@@ -9646,13 +9654,13 @@
       <c r="J106" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="K106" s="27">
+      <c r="K106" s="30">
         <v>1.00000250000625</v>
       </c>
-      <c r="L106" s="28">
+      <c r="L106" s="31">
         <v>1.414220633467423E-6</v>
       </c>
-      <c r="M106" s="29">
+      <c r="M106" s="32">
         <v>120.87512900978579</v>
       </c>
       <c r="N106" s="14" t="s">
@@ -9669,13 +9677,13 @@
       <c r="J107" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="K107" s="30">
+      <c r="K107" s="27">
         <v>1.0000031000096099</v>
       </c>
-      <c r="L107" s="31">
+      <c r="L107" s="28">
         <v>9.1924451484967022E-7</v>
       </c>
-      <c r="M107" s="32">
+      <c r="M107" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N107" s="9" t="s">
@@ -9692,13 +9700,13 @@
       <c r="J108" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="K108" s="30">
+      <c r="K108" s="27">
         <v>1.000003050009302</v>
       </c>
-      <c r="L108" s="31">
+      <c r="L108" s="28">
         <v>7.0711109455764635E-7</v>
       </c>
-      <c r="M108" s="32">
+      <c r="M108" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N108" s="9" t="s">
@@ -9715,13 +9723,13 @@
       <c r="J109" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="K109" s="30">
+      <c r="K109" s="27">
         <v>1.000003250010562</v>
       </c>
-      <c r="L109" s="31">
+      <c r="L109" s="28">
         <v>8.1317808401348648E-7</v>
       </c>
-      <c r="M109" s="32">
+      <c r="M109" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N109" s="9" t="s">
@@ -9738,13 +9746,13 @@
       <c r="J110" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="K110" s="30">
+      <c r="K110" s="27">
         <v>1.0000034000115601</v>
       </c>
-      <c r="L110" s="31">
+      <c r="L110" s="28">
         <v>3.5355579476859112E-7</v>
       </c>
-      <c r="M110" s="32">
+      <c r="M110" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N110" s="9" t="s">
@@ -9761,13 +9769,13 @@
       <c r="J111" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="K111" s="30">
+      <c r="K111" s="27">
         <v>1.0000033000108901</v>
       </c>
-      <c r="L111" s="31">
+      <c r="L111" s="28">
         <v>2.4748900684004159E-7</v>
       </c>
-      <c r="M111" s="32">
+      <c r="M111" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N111" s="9" t="s">
@@ -9784,13 +9792,13 @@
       <c r="J112" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="K112" s="27">
+      <c r="K112" s="30">
         <v>1.0000029000084101</v>
       </c>
-      <c r="L112" s="28">
+      <c r="L112" s="31">
         <v>8.4853305890846271E-7</v>
       </c>
-      <c r="M112" s="29">
+      <c r="M112" s="32">
         <v>120.87512900978579</v>
       </c>
       <c r="N112" s="14" t="s">
@@ -9807,13 +9815,13 @@
       <c r="J113" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="K113" s="30">
+      <c r="K113" s="27">
         <v>1.000002750007563</v>
       </c>
-      <c r="L113" s="31">
+      <c r="L113" s="28">
         <v>7.0711067028988679E-7</v>
       </c>
-      <c r="M113" s="32">
+      <c r="M113" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N113" s="9" t="s">
@@ -9836,7 +9844,7 @@
       <c r="L114" s="34">
         <v>2E-8</v>
       </c>
-      <c r="M114" s="32">
+      <c r="M114" s="29">
         <v>18</v>
       </c>
       <c r="N114" s="9" t="s">
@@ -9859,7 +9867,7 @@
       <c r="L115" s="34">
         <v>2E-8</v>
       </c>
-      <c r="M115" s="32">
+      <c r="M115" s="29">
         <v>18</v>
       </c>
       <c r="N115" s="9" t="s">
@@ -10004,13 +10012,13 @@
       <c r="J124" s="21" t="s">
         <v>442</v>
       </c>
-      <c r="K124" s="30">
+      <c r="K124" s="27">
         <v>1.00000250000625</v>
       </c>
-      <c r="L124" s="31">
+      <c r="L124" s="28">
         <v>1.4142206334674234E-6</v>
       </c>
-      <c r="M124" s="32">
+      <c r="M124" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N124" s="9" t="s">
@@ -10030,10 +10038,10 @@
       <c r="K125" s="37">
         <v>1</v>
       </c>
-      <c r="L125" s="28">
+      <c r="L125" s="31">
         <v>1.4142135623730949E-6</v>
       </c>
-      <c r="M125" s="29">
+      <c r="M125" s="32">
         <v>120.87512900978579</v>
       </c>
       <c r="N125" s="14" t="s">
@@ -10050,13 +10058,13 @@
       <c r="J126" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="K126" s="30">
+      <c r="K126" s="27">
         <v>1.00000150000225</v>
       </c>
-      <c r="L126" s="31">
+      <c r="L126" s="28">
         <v>9.1924157326516319E-7</v>
       </c>
-      <c r="M126" s="32">
+      <c r="M126" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N126" s="9" t="s">
@@ -10073,13 +10081,13 @@
       <c r="J127" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="K127" s="30">
+      <c r="K127" s="27">
         <v>1.00000160000256</v>
       </c>
-      <c r="L127" s="31">
+      <c r="L127" s="28">
         <v>7.0710904393367791E-7</v>
       </c>
-      <c r="M127" s="32">
+      <c r="M127" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N127" s="9" t="s">
@@ -10096,13 +10104,13 @@
       <c r="J128" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="K128" s="30">
+      <c r="K128" s="27">
         <v>1.000001550002402</v>
       </c>
-      <c r="L128" s="31">
+      <c r="L128" s="28">
         <v>8.1317531920606548E-7</v>
       </c>
-      <c r="M128" s="32">
+      <c r="M128" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N128" s="9" t="s">
@@ -10119,13 +10127,13 @@
       <c r="J129" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="K129" s="30">
+      <c r="K129" s="27">
         <v>1.00000170000289</v>
       </c>
-      <c r="L129" s="31">
+      <c r="L129" s="28">
         <v>3.5355459267786709E-7</v>
       </c>
-      <c r="M129" s="32">
+      <c r="M129" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N129" s="9" t="s">
@@ -10142,13 +10150,13 @@
       <c r="J130" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="K130" s="30">
+      <c r="K130" s="27">
         <v>1.000001850003422</v>
       </c>
-      <c r="L130" s="31">
+      <c r="L130" s="28">
         <v>2.4748828912111432E-7</v>
       </c>
-      <c r="M130" s="32">
+      <c r="M130" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N130" s="9" t="s">
@@ -10165,13 +10173,13 @@
       <c r="J131" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="K131" s="27">
+      <c r="K131" s="30">
         <v>1.00000180000324</v>
       </c>
-      <c r="L131" s="28">
+      <c r="L131" s="31">
         <v>8.4853119213339951E-7</v>
       </c>
-      <c r="M131" s="29">
+      <c r="M131" s="32">
         <v>120.87512900978579</v>
       </c>
       <c r="N131" s="14" t="s">
@@ -10188,13 +10196,13 @@
       <c r="J132" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="K132" s="30">
+      <c r="K132" s="27">
         <v>1.000001750003062</v>
       </c>
-      <c r="L132" s="31">
+      <c r="L132" s="28">
         <v>7.0710925606677826E-7</v>
       </c>
-      <c r="M132" s="32">
+      <c r="M132" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N132" s="9" t="s">
@@ -10217,7 +10225,7 @@
       <c r="L133" s="34">
         <v>1.9000000000000001E-8</v>
       </c>
-      <c r="M133" s="32">
+      <c r="M133" s="29">
         <v>18</v>
       </c>
       <c r="N133" s="9" t="s">
@@ -10240,7 +10248,7 @@
       <c r="L134" s="34">
         <v>1.9000000000000001E-8</v>
       </c>
-      <c r="M134" s="32">
+      <c r="M134" s="29">
         <v>18</v>
       </c>
       <c r="N134" s="9" t="s">
@@ -10385,13 +10393,13 @@
       <c r="J143" s="21" t="s">
         <v>442</v>
       </c>
-      <c r="K143" s="30">
+      <c r="K143" s="27">
         <v>1</v>
       </c>
-      <c r="L143" s="31">
+      <c r="L143" s="28">
         <v>1.4142135623730949E-6</v>
       </c>
-      <c r="M143" s="32">
+      <c r="M143" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N143" s="9" t="s">
@@ -10411,10 +10419,10 @@
       <c r="K144" s="37">
         <v>1</v>
       </c>
-      <c r="L144" s="28">
+      <c r="L144" s="31">
         <v>1.4142135623730949E-6</v>
       </c>
-      <c r="M144" s="29">
+      <c r="M144" s="32">
         <v>120.87512900978579</v>
       </c>
       <c r="N144" s="14" t="s">
@@ -10431,13 +10439,13 @@
       <c r="J145" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="K145" s="30">
+      <c r="K145" s="27">
         <v>1.00000150000225</v>
       </c>
-      <c r="L145" s="31">
+      <c r="L145" s="28">
         <v>9.1924157326516319E-7</v>
       </c>
-      <c r="M145" s="32">
+      <c r="M145" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N145" s="9" t="s">
@@ -10454,13 +10462,13 @@
       <c r="J146" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="K146" s="30">
+      <c r="K146" s="27">
         <v>1.00000160000256</v>
       </c>
-      <c r="L146" s="31">
+      <c r="L146" s="28">
         <v>7.0710904393367791E-7</v>
       </c>
-      <c r="M146" s="32">
+      <c r="M146" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N146" s="9" t="s">
@@ -10477,13 +10485,13 @@
       <c r="J147" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="K147" s="30">
+      <c r="K147" s="27">
         <v>1.000009650093123</v>
       </c>
-      <c r="L147" s="31">
+      <c r="L147" s="28">
         <v>8.1318849282671504E-7</v>
       </c>
-      <c r="M147" s="32">
+      <c r="M147" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N147" s="9" t="s">
@@ -10500,13 +10508,13 @@
       <c r="J148" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="K148" s="30">
+      <c r="K148" s="27">
         <v>1.00000170000289</v>
       </c>
-      <c r="L148" s="31">
+      <c r="L148" s="28">
         <v>3.5355459267786709E-7</v>
       </c>
-      <c r="M148" s="32">
+      <c r="M148" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N148" s="9" t="s">
@@ -10523,13 +10531,13 @@
       <c r="J149" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="K149" s="30">
+      <c r="K149" s="27">
         <v>1.000001850003422</v>
       </c>
-      <c r="L149" s="31">
+      <c r="L149" s="28">
         <v>2.4748828912111432E-7</v>
       </c>
-      <c r="M149" s="32">
+      <c r="M149" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N149" s="9" t="s">
@@ -10546,13 +10554,13 @@
       <c r="J150" s="21" t="s">
         <v>330</v>
       </c>
-      <c r="K150" s="27">
+      <c r="K150" s="30">
         <v>1.00000180000324</v>
       </c>
-      <c r="L150" s="28">
+      <c r="L150" s="31">
         <v>8.4853119213339951E-7</v>
       </c>
-      <c r="M150" s="29">
+      <c r="M150" s="32">
         <v>120.87512900978579</v>
       </c>
       <c r="N150" s="14" t="s">
@@ -10569,13 +10577,13 @@
       <c r="J151" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="K151" s="30">
+      <c r="K151" s="27">
         <v>1.000001750003062</v>
       </c>
-      <c r="L151" s="31">
+      <c r="L151" s="28">
         <v>7.0710925606677826E-7</v>
       </c>
-      <c r="M151" s="32">
+      <c r="M151" s="29">
         <v>120.87512900978579</v>
       </c>
       <c r="N151" s="9" t="s">
@@ -10598,7 +10606,7 @@
       <c r="L152" s="34">
         <v>1.7E-8</v>
       </c>
-      <c r="M152" s="32">
+      <c r="M152" s="29">
         <v>18</v>
       </c>
       <c r="N152" s="9" t="s">
@@ -10621,7 +10629,7 @@
       <c r="L153" s="34">
         <v>1.7E-8</v>
       </c>
-      <c r="M153" s="32">
+      <c r="M153" s="29">
         <v>18</v>
       </c>
       <c r="N153" s="9" t="s">

</xml_diff>